<commit_message>
Add codes for Supplier Certificate and resolved some issues
</commit_message>
<xml_diff>
--- a/Docs/Testing Issue List.xlsx
+++ b/Docs/Testing Issue List.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Zhongding.git\trunk\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>#</t>
   </si>
@@ -42,9 +47,6 @@
     <t>帐套管理 列表的列与页面设计不一致</t>
   </si>
   <si>
-    <t>帐套的排序，现在是按帐套编号倒序，改成升序吧。</t>
-  </si>
-  <si>
     <t>新建一个帐套时，维护页面的删除按钮应该隐藏或灰掉，现在点击删除，页面没有反应。</t>
   </si>
   <si>
@@ -52,9 +54,6 @@
   </si>
   <si>
     <t>银行帐号管理</t>
-  </si>
-  <si>
-    <t>列表查询条件，去掉帐套，因为当前页面只能显示当前帐套和所有的私人账户。</t>
   </si>
   <si>
     <t>列表只需要保留如下列：
@@ -62,24 +61,42 @@
 且账号，不需要加***</t>
   </si>
   <si>
+    <t>待解决</t>
+  </si>
+  <si>
+    <t>帐套的排序，现在是按帐套编号倒序，改成升序吧。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>已解决</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>列表查询条件，去掉帐套，因为当前页面只能显示当前帐套和所有的私人账户。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>维护页面的备注输入框，不支持copy/paste， 需要看看是什么原因</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>帐号的正则表达式验证，能不能多支持一种以空格分隔的？ 如 4225 5555 2222 5555 235</t>
-  </si>
-  <si>
-    <t>待解决</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -104,13 +121,32 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -140,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -179,15 +215,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -427,7 +472,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -469,7 +514,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -504,7 +549,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -716,19 +761,19 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="51.85546875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="22.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="51.875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
@@ -760,10 +805,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E2" s="11">
         <v>41950</v>
@@ -781,8 +826,8 @@
       <c r="C3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>16</v>
+      <c r="D3" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="E3" s="11">
         <v>41950</v>
@@ -798,10 +843,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="E4" s="11">
         <v>41950</v>
@@ -817,10 +862,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="E5" s="11">
         <v>41950</v>
@@ -833,13 +878,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="E6" s="11">
         <v>41950</v>
@@ -852,13 +897,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>16</v>
+      <c r="D7" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="E7" s="11">
         <v>41950</v>
@@ -871,30 +916,30 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="9" t="s">
         <v>16</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>18</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" ht="49.5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A9" s="13">
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
@@ -1207,6 +1252,7 @@
       <c r="G43" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1219,8 +1265,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1231,8 +1278,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Resolved some issues opened on 2014/11/10
</commit_message>
<xml_diff>
--- a/Docs/Testing Issue List.xlsx
+++ b/Docs/Testing Issue List.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Zhongding.git\trunk\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="195" windowWidth="20115" windowHeight="7875"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t>#</t>
   </si>
@@ -109,17 +114,25 @@
   </si>
   <si>
     <t>供应商列表的删除功能不好用。</t>
+  </si>
+  <si>
+    <t>已解决</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>已解决</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -146,7 +159,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -235,7 +248,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -446,7 +459,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -488,7 +501,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -523,7 +536,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -734,23 +747,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="20" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="51.85546875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="22.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18.75" style="20" customWidth="1"/>
+    <col min="5" max="5" width="15.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="51.875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -771,7 +784,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="133.5" customHeight="1">
+    <row r="2" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -790,7 +803,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" ht="16.5">
+    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -809,7 +822,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" ht="191.25" customHeight="1">
+    <row r="4" spans="1:7" ht="191.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -828,7 +841,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7" ht="74.25" customHeight="1">
+    <row r="5" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -847,7 +860,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:7" ht="217.5" customHeight="1">
+    <row r="6" spans="1:7" ht="217.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -866,7 +879,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7" ht="172.5" customHeight="1">
+    <row r="7" spans="1:7" ht="172.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -885,7 +898,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7" ht="243.75" customHeight="1">
+    <row r="8" spans="1:7" ht="243.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -902,7 +915,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" ht="49.5">
+    <row r="9" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A9" s="13">
         <v>8</v>
       </c>
@@ -919,7 +932,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" ht="16.5">
+    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A10" s="13"/>
       <c r="B10" s="9" t="s">
         <v>19</v>
@@ -928,15 +941,17 @@
         <v>20</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E10" s="11">
         <v>41953</v>
       </c>
-      <c r="F10" s="9"/>
+      <c r="F10" s="11">
+        <v>41954</v>
+      </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" ht="16.5">
+    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A11" s="13"/>
       <c r="B11" s="9" t="s">
         <v>19</v>
@@ -945,15 +960,17 @@
         <v>21</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E11" s="11">
         <v>41953</v>
       </c>
-      <c r="F11" s="9"/>
+      <c r="F11" s="11">
+        <v>41955</v>
+      </c>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7" ht="33">
+    <row r="12" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A12" s="13"/>
       <c r="B12" s="9" t="s">
         <v>19</v>
@@ -962,15 +979,17 @@
         <v>22</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E12" s="11">
         <v>41953</v>
       </c>
-      <c r="F12" s="9"/>
+      <c r="F12" s="11">
+        <v>41954</v>
+      </c>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:7" ht="33">
+    <row r="13" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A13" s="13"/>
       <c r="B13" s="9" t="s">
         <v>19</v>
@@ -979,15 +998,17 @@
         <v>23</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E13" s="11">
         <v>41953</v>
       </c>
-      <c r="F13" s="9"/>
+      <c r="F13" s="11">
+        <v>41954</v>
+      </c>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:7" ht="66">
+    <row r="14" spans="1:7" ht="66" x14ac:dyDescent="0.15">
       <c r="A14" s="13"/>
       <c r="B14" s="9" t="s">
         <v>19</v>
@@ -996,15 +1017,17 @@
         <v>25</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E14" s="11">
         <v>41953</v>
       </c>
-      <c r="F14" s="9"/>
+      <c r="F14" s="11">
+        <v>41955</v>
+      </c>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:7" ht="33">
+    <row r="15" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A15" s="13"/>
       <c r="B15" s="9" t="s">
         <v>19</v>
@@ -1013,15 +1036,17 @@
         <v>24</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="E15" s="11">
         <v>41953</v>
       </c>
-      <c r="F15" s="9"/>
+      <c r="F15" s="11">
+        <v>41954</v>
+      </c>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" ht="16.5">
+    <row r="16" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A16" s="13"/>
       <c r="B16" s="9" t="s">
         <v>19</v>
@@ -1030,15 +1055,17 @@
         <v>26</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E16" s="11">
         <v>41953</v>
       </c>
-      <c r="F16" s="9"/>
+      <c r="F16" s="11">
+        <v>41955</v>
+      </c>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="1:7" ht="16.5">
+    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A17" s="13"/>
       <c r="B17" s="9"/>
       <c r="C17" s="10"/>
@@ -1047,7 +1074,7 @@
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" ht="16.5">
+    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A18" s="13"/>
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
@@ -1056,7 +1083,7 @@
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
     </row>
-    <row r="19" spans="1:7" ht="16.5">
+    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A19" s="13"/>
       <c r="B19" s="9"/>
       <c r="C19" s="10"/>
@@ -1065,7 +1092,7 @@
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="1:7" ht="16.5">
+    <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A20" s="13"/>
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
@@ -1074,7 +1101,7 @@
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="1:7" ht="16.5">
+    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A21" s="13"/>
       <c r="B21" s="9"/>
       <c r="C21" s="10"/>
@@ -1083,7 +1110,7 @@
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
     </row>
-    <row r="22" spans="1:7" ht="16.5">
+    <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A22" s="13"/>
       <c r="B22" s="9"/>
       <c r="C22" s="10"/>
@@ -1092,7 +1119,7 @@
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
     </row>
-    <row r="23" spans="1:7" ht="16.5">
+    <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A23" s="13"/>
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
@@ -1101,7 +1128,7 @@
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
     </row>
-    <row r="24" spans="1:7" ht="16.5">
+    <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A24" s="13"/>
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
@@ -1110,7 +1137,7 @@
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="1:7" ht="16.5">
+    <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A25" s="13"/>
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
@@ -1119,7 +1146,7 @@
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
     </row>
-    <row r="26" spans="1:7" ht="16.5">
+    <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A26" s="13"/>
       <c r="B26" s="9"/>
       <c r="C26" s="10"/>
@@ -1128,7 +1155,7 @@
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="1:7" ht="16.5">
+    <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A27" s="13"/>
       <c r="B27" s="9"/>
       <c r="C27" s="10"/>
@@ -1137,7 +1164,7 @@
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="1:7" ht="16.5">
+    <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A28" s="13"/>
       <c r="B28" s="9"/>
       <c r="C28" s="10"/>
@@ -1146,7 +1173,7 @@
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="1:7" ht="16.5">
+    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A29" s="13"/>
       <c r="B29" s="9"/>
       <c r="C29" s="10"/>
@@ -1155,7 +1182,7 @@
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="1:7" ht="16.5">
+    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A30" s="13"/>
       <c r="B30" s="9"/>
       <c r="C30" s="10"/>
@@ -1164,7 +1191,7 @@
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
     </row>
-    <row r="31" spans="1:7" ht="16.5">
+    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A31" s="13"/>
       <c r="B31" s="9"/>
       <c r="C31" s="10"/>
@@ -1173,7 +1200,7 @@
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
     </row>
-    <row r="32" spans="1:7" ht="16.5">
+    <row r="32" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A32" s="13"/>
       <c r="B32" s="9"/>
       <c r="C32" s="10"/>
@@ -1182,7 +1209,7 @@
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
     </row>
-    <row r="33" spans="1:7" ht="16.5">
+    <row r="33" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A33" s="13"/>
       <c r="B33" s="9"/>
       <c r="C33" s="10"/>
@@ -1191,7 +1218,7 @@
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
     </row>
-    <row r="34" spans="1:7" ht="16.5">
+    <row r="34" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A34" s="13"/>
       <c r="B34" s="9"/>
       <c r="C34" s="10"/>
@@ -1200,7 +1227,7 @@
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
     </row>
-    <row r="35" spans="1:7" ht="16.5">
+    <row r="35" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
       <c r="B35" s="3"/>
       <c r="C35" s="6"/>
@@ -1209,7 +1236,7 @@
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" ht="16.5">
+    <row r="36" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A36" s="13"/>
       <c r="B36" s="3"/>
       <c r="C36" s="6"/>
@@ -1218,7 +1245,7 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" ht="16.5">
+    <row r="37" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A37" s="13"/>
       <c r="B37" s="3"/>
       <c r="C37" s="6"/>
@@ -1227,7 +1254,7 @@
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="1:7" ht="16.5">
+    <row r="38" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A38" s="13"/>
       <c r="B38" s="3"/>
       <c r="C38" s="6"/>
@@ -1236,7 +1263,7 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" ht="16.5">
+    <row r="39" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A39" s="13"/>
       <c r="B39" s="3"/>
       <c r="C39" s="6"/>
@@ -1245,7 +1272,7 @@
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:7" ht="16.5">
+    <row r="40" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A40" s="13"/>
       <c r="B40" s="3"/>
       <c r="C40" s="6"/>
@@ -1254,7 +1281,7 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41" s="14"/>
       <c r="B41" s="4"/>
       <c r="C41" s="7"/>
@@ -1263,7 +1290,7 @@
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42" s="12"/>
       <c r="B42" s="2"/>
       <c r="C42" s="5"/>
@@ -1287,7 +1314,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1300,7 +1327,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Check in database changes
</commit_message>
<xml_diff>
--- a/Docs/Testing Issue List.xlsx
+++ b/Docs/Testing Issue List.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Zhongding.git\trunk\Docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="195" windowWidth="20115" windowHeight="7875"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
   <si>
     <t>#</t>
   </si>
@@ -116,23 +111,24 @@
     <t>供应商列表的删除功能不好用。</t>
   </si>
   <si>
-    <t>已解决</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>已解决</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <t>highlighted Grid header是否可以不换行？</t>
+  </si>
+  <si>
+    <t>测试通过</t>
+  </si>
+  <si>
+    <t>所有的grid 的排序功能，列明不要换行</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -159,7 +155,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -248,7 +244,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -455,11 +451,87 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>227404</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>2287161</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7886700" y="16935450"/>
+          <a:ext cx="9104704" cy="2201436"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>189215</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>2577870</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7981950" y="19297650"/>
+          <a:ext cx="9580865" cy="2501670"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -501,7 +573,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -536,7 +608,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -747,23 +819,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.125" style="15" customWidth="1"/>
-    <col min="2" max="2" width="22.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="18.75" style="20" customWidth="1"/>
-    <col min="5" max="5" width="15.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="51.875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.125" style="1"/>
+    <col min="1" max="1" width="11.140625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="20" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="51.85546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -784,7 +856,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="133.5" customHeight="1">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -803,7 +875,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="16.5">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -814,7 +886,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E3" s="11">
         <v>41950</v>
@@ -822,7 +894,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" ht="191.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="191.25" customHeight="1">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -841,7 +913,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="74.25" customHeight="1">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -860,7 +932,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:7" ht="217.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="217.5" customHeight="1">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -879,7 +951,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7" ht="172.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="172.5" customHeight="1">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -898,7 +970,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7" ht="243.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="243.75" customHeight="1">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -915,7 +987,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" ht="33" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="49.5">
       <c r="A9" s="13">
         <v>8</v>
       </c>
@@ -932,7 +1004,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="16.5">
       <c r="A10" s="13"/>
       <c r="B10" s="9" t="s">
         <v>19</v>
@@ -941,7 +1013,7 @@
         <v>20</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E10" s="11">
         <v>41953</v>
@@ -951,7 +1023,7 @@
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="16.5">
       <c r="A11" s="13"/>
       <c r="B11" s="9" t="s">
         <v>19</v>
@@ -960,7 +1032,7 @@
         <v>21</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E11" s="11">
         <v>41953</v>
@@ -970,7 +1042,7 @@
       </c>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7" ht="33" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="33">
       <c r="A12" s="13"/>
       <c r="B12" s="9" t="s">
         <v>19</v>
@@ -979,7 +1051,7 @@
         <v>22</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E12" s="11">
         <v>41953</v>
@@ -989,7 +1061,7 @@
       </c>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:7" ht="33" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="33">
       <c r="A13" s="13"/>
       <c r="B13" s="9" t="s">
         <v>19</v>
@@ -998,7 +1070,7 @@
         <v>23</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E13" s="11">
         <v>41953</v>
@@ -1008,7 +1080,7 @@
       </c>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:7" ht="66" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="66">
       <c r="A14" s="13"/>
       <c r="B14" s="9" t="s">
         <v>19</v>
@@ -1017,7 +1089,7 @@
         <v>25</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E14" s="11">
         <v>41953</v>
@@ -1027,7 +1099,7 @@
       </c>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:7" ht="33" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="33">
       <c r="A15" s="13"/>
       <c r="B15" s="9" t="s">
         <v>19</v>
@@ -1046,7 +1118,7 @@
       </c>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="16.5">
       <c r="A16" s="13"/>
       <c r="B16" s="9" t="s">
         <v>19</v>
@@ -1055,7 +1127,7 @@
         <v>26</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E16" s="11">
         <v>41953</v>
@@ -1065,25 +1137,43 @@
       </c>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="186.75" customHeight="1">
       <c r="A17" s="13"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="9"/>
+      <c r="B17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="11">
+        <v>41956</v>
+      </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="216.75" customHeight="1">
       <c r="A18" s="13"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="B18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="11">
+        <v>41956</v>
+      </c>
+      <c r="F18" s="11">
+        <v>41956</v>
+      </c>
       <c r="G18" s="9"/>
     </row>
-    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="16.5">
       <c r="A19" s="13"/>
       <c r="B19" s="9"/>
       <c r="C19" s="10"/>
@@ -1092,7 +1182,7 @@
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="16.5">
       <c r="A20" s="13"/>
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
@@ -1101,7 +1191,7 @@
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="16.5">
       <c r="A21" s="13"/>
       <c r="B21" s="9"/>
       <c r="C21" s="10"/>
@@ -1110,7 +1200,7 @@
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
     </row>
-    <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="16.5">
       <c r="A22" s="13"/>
       <c r="B22" s="9"/>
       <c r="C22" s="10"/>
@@ -1119,7 +1209,7 @@
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
     </row>
-    <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="16.5">
       <c r="A23" s="13"/>
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
@@ -1128,7 +1218,7 @@
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
     </row>
-    <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="16.5">
       <c r="A24" s="13"/>
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
@@ -1137,7 +1227,7 @@
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="16.5">
       <c r="A25" s="13"/>
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
@@ -1146,7 +1236,7 @@
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
     </row>
-    <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="16.5">
       <c r="A26" s="13"/>
       <c r="B26" s="9"/>
       <c r="C26" s="10"/>
@@ -1155,7 +1245,7 @@
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="16.5">
       <c r="A27" s="13"/>
       <c r="B27" s="9"/>
       <c r="C27" s="10"/>
@@ -1164,7 +1254,7 @@
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" ht="16.5">
       <c r="A28" s="13"/>
       <c r="B28" s="9"/>
       <c r="C28" s="10"/>
@@ -1173,7 +1263,7 @@
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" ht="16.5">
       <c r="A29" s="13"/>
       <c r="B29" s="9"/>
       <c r="C29" s="10"/>
@@ -1182,7 +1272,7 @@
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:7" ht="16.5">
       <c r="A30" s="13"/>
       <c r="B30" s="9"/>
       <c r="C30" s="10"/>
@@ -1191,7 +1281,7 @@
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
     </row>
-    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:7" ht="16.5">
       <c r="A31" s="13"/>
       <c r="B31" s="9"/>
       <c r="C31" s="10"/>
@@ -1200,7 +1290,7 @@
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
     </row>
-    <row r="32" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:7" ht="16.5">
       <c r="A32" s="13"/>
       <c r="B32" s="9"/>
       <c r="C32" s="10"/>
@@ -1209,7 +1299,7 @@
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
     </row>
-    <row r="33" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:7" ht="16.5">
       <c r="A33" s="13"/>
       <c r="B33" s="9"/>
       <c r="C33" s="10"/>
@@ -1218,7 +1308,7 @@
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
     </row>
-    <row r="34" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:7" ht="16.5">
       <c r="A34" s="13"/>
       <c r="B34" s="9"/>
       <c r="C34" s="10"/>
@@ -1227,7 +1317,7 @@
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
     </row>
-    <row r="35" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="16.5">
       <c r="A35" s="13"/>
       <c r="B35" s="3"/>
       <c r="C35" s="6"/>
@@ -1236,7 +1326,7 @@
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="16.5">
       <c r="A36" s="13"/>
       <c r="B36" s="3"/>
       <c r="C36" s="6"/>
@@ -1245,7 +1335,7 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="16.5">
       <c r="A37" s="13"/>
       <c r="B37" s="3"/>
       <c r="C37" s="6"/>
@@ -1254,7 +1344,7 @@
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="16.5">
       <c r="A38" s="13"/>
       <c r="B38" s="3"/>
       <c r="C38" s="6"/>
@@ -1263,7 +1353,7 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="16.5">
       <c r="A39" s="13"/>
       <c r="B39" s="3"/>
       <c r="C39" s="6"/>
@@ -1272,7 +1362,7 @@
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="16.5">
       <c r="A40" s="13"/>
       <c r="B40" s="3"/>
       <c r="C40" s="6"/>
@@ -1281,7 +1371,7 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:7">
       <c r="A41" s="14"/>
       <c r="B41" s="4"/>
       <c r="C41" s="7"/>
@@ -1290,7 +1380,7 @@
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:7">
       <c r="A42" s="12"/>
       <c r="B42" s="2"/>
       <c r="C42" s="5"/>
@@ -1314,7 +1404,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1327,7 +1417,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add codes for product price manage and resolved some issues
</commit_message>
<xml_diff>
--- a/Docs/Testing Issue List.xlsx
+++ b/Docs/Testing Issue List.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Zhongding.git\trunk\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="195" windowWidth="20115" windowHeight="7875"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
   <si>
     <t>#</t>
   </si>
@@ -57,9 +62,6 @@
     <t>列表只需要保留如下列：
 户名，开户行，帐号，类别，备注
 且账号，不需要加***</t>
-  </si>
-  <si>
-    <t>待解决</t>
   </si>
   <si>
     <t>帐套的排序，现在是按帐套编号倒序，改成升序吧。</t>
@@ -136,17 +138,33 @@
 把商业单位放到第二行，宽度加宽
 名称 列改为：客户名称 （Grid上也改掉）
 客户名称查询也应该使用dropdown 控件</t>
+  </si>
+  <si>
+    <t>已解决</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>已解决</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>已解决</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -173,7 +191,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -262,7 +280,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -611,8 +629,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7848600" y="24705238"/>
-          <a:ext cx="6980770" cy="2040654"/>
+          <a:off x="8972550" y="24495688"/>
+          <a:ext cx="7904695" cy="2040654"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -663,7 +681,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -705,7 +723,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -740,7 +758,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -951,23 +969,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="20" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="51.85546875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="22.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18.75" style="20" customWidth="1"/>
+    <col min="5" max="5" width="15.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="51.875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -988,7 +1007,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="133.5" customHeight="1">
+    <row r="2" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -999,7 +1018,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="E2" s="11">
         <v>41950</v>
@@ -1007,7 +1026,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" ht="16.5">
+    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -1018,7 +1037,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="11">
         <v>41950</v>
@@ -1026,7 +1045,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" ht="191.25" customHeight="1">
+    <row r="4" spans="1:7" ht="191.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -1034,10 +1053,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>14</v>
       </c>
       <c r="E4" s="11">
         <v>41950</v>
@@ -1045,7 +1064,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7" ht="74.25" customHeight="1">
+    <row r="5" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -1056,7 +1075,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="11">
         <v>41950</v>
@@ -1064,7 +1083,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:7" ht="217.5" customHeight="1">
+    <row r="6" spans="1:7" ht="217.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -1072,10 +1091,10 @@
         <v>10</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="11">
         <v>41950</v>
@@ -1083,7 +1102,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7" ht="172.5" customHeight="1">
+    <row r="7" spans="1:7" ht="172.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -1094,7 +1113,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" s="11">
         <v>41950</v>
@@ -1102,7 +1121,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7" ht="243.75" customHeight="1">
+    <row r="8" spans="1:7" ht="243.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -1110,16 +1129,16 @@
         <v>10</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" ht="49.5">
+    <row r="9" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A9" s="13">
         <v>8</v>
       </c>
@@ -1127,25 +1146,25 @@
         <v>10</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" ht="16.5">
+    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A10" s="13"/>
       <c r="B10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>20</v>
-      </c>
       <c r="D10" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" s="11">
         <v>41953</v>
@@ -1155,16 +1174,16 @@
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" ht="16.5">
+    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A11" s="13"/>
       <c r="B11" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" s="11">
         <v>41953</v>
@@ -1174,16 +1193,16 @@
       </c>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7" ht="33">
+    <row r="12" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A12" s="13"/>
       <c r="B12" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" s="11">
         <v>41953</v>
@@ -1193,16 +1212,16 @@
       </c>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:7" ht="33">
+    <row r="13" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A13" s="13"/>
       <c r="B13" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" s="11">
         <v>41953</v>
@@ -1212,16 +1231,16 @@
       </c>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:7" ht="66">
+    <row r="14" spans="1:7" ht="66" x14ac:dyDescent="0.15">
       <c r="A14" s="13"/>
       <c r="B14" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E14" s="11">
         <v>41953</v>
@@ -1231,16 +1250,16 @@
       </c>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:7" ht="33">
+    <row r="15" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A15" s="13"/>
       <c r="B15" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" s="11">
         <v>41953</v>
@@ -1250,16 +1269,16 @@
       </c>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" ht="16.5">
+    <row r="16" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A16" s="13"/>
       <c r="B16" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E16" s="11">
         <v>41953</v>
@@ -1269,33 +1288,35 @@
       </c>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="1:7" ht="186.75" customHeight="1">
+    <row r="17" spans="1:7" ht="186.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13"/>
       <c r="B17" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="E17" s="11">
         <v>41956</v>
       </c>
-      <c r="F17" s="9"/>
+      <c r="F17" s="11">
+        <v>41963</v>
+      </c>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" ht="216.75" customHeight="1">
+    <row r="18" spans="1:7" ht="216.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="13"/>
       <c r="B18" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" s="11">
         <v>41956</v>
@@ -1305,63 +1326,75 @@
       </c>
       <c r="G18" s="9"/>
     </row>
-    <row r="19" spans="1:7" ht="16.5">
+    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A19" s="13"/>
       <c r="B19" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>31</v>
-      </c>
       <c r="D19" s="17" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="E19" s="11">
         <v>41962</v>
       </c>
-      <c r="F19" s="9"/>
+      <c r="F19" s="11">
+        <v>41964</v>
+      </c>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="1:7" ht="199.5" customHeight="1">
+    <row r="20" spans="1:7" ht="199.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13"/>
       <c r="B20" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="17"/>
+        <v>26</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
+      <c r="F20" s="11">
+        <v>41963</v>
+      </c>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="1:7" ht="163.5" customHeight="1">
+    <row r="21" spans="1:7" ht="163.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="13"/>
       <c r="B21" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="17"/>
+      <c r="D21" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
+      <c r="F21" s="11">
+        <v>41963</v>
+      </c>
       <c r="G21" s="9"/>
     </row>
-    <row r="22" spans="1:7" ht="162" customHeight="1">
+    <row r="22" spans="1:7" ht="162" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="13"/>
       <c r="B22" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="17"/>
+        <v>33</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>37</v>
+      </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
     </row>
-    <row r="23" spans="1:7" ht="16.5">
+    <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A23" s="13"/>
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
@@ -1370,7 +1403,7 @@
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
     </row>
-    <row r="24" spans="1:7" ht="16.5">
+    <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A24" s="13"/>
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
@@ -1379,7 +1412,7 @@
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="1:7" ht="16.5">
+    <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A25" s="13"/>
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
@@ -1388,7 +1421,7 @@
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
     </row>
-    <row r="26" spans="1:7" ht="16.5">
+    <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A26" s="13"/>
       <c r="B26" s="9"/>
       <c r="C26" s="10"/>
@@ -1397,7 +1430,7 @@
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="1:7" ht="16.5">
+    <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A27" s="13"/>
       <c r="B27" s="9"/>
       <c r="C27" s="10"/>
@@ -1406,7 +1439,7 @@
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="1:7" ht="16.5">
+    <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A28" s="13"/>
       <c r="B28" s="9"/>
       <c r="C28" s="10"/>
@@ -1415,7 +1448,7 @@
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="1:7" ht="16.5">
+    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A29" s="13"/>
       <c r="B29" s="9"/>
       <c r="C29" s="10"/>
@@ -1424,7 +1457,7 @@
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="1:7" ht="16.5">
+    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A30" s="13"/>
       <c r="B30" s="9"/>
       <c r="C30" s="10"/>
@@ -1433,7 +1466,7 @@
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
     </row>
-    <row r="31" spans="1:7" ht="16.5">
+    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A31" s="13"/>
       <c r="B31" s="9"/>
       <c r="C31" s="10"/>
@@ -1442,7 +1475,7 @@
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
     </row>
-    <row r="32" spans="1:7" ht="16.5">
+    <row r="32" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A32" s="13"/>
       <c r="B32" s="9"/>
       <c r="C32" s="10"/>
@@ -1451,7 +1484,7 @@
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
     </row>
-    <row r="33" spans="1:7" ht="16.5">
+    <row r="33" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A33" s="13"/>
       <c r="B33" s="9"/>
       <c r="C33" s="10"/>
@@ -1460,7 +1493,7 @@
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
     </row>
-    <row r="34" spans="1:7" ht="16.5">
+    <row r="34" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A34" s="13"/>
       <c r="B34" s="9"/>
       <c r="C34" s="10"/>
@@ -1469,7 +1502,7 @@
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
     </row>
-    <row r="35" spans="1:7" ht="16.5">
+    <row r="35" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
       <c r="B35" s="3"/>
       <c r="C35" s="6"/>
@@ -1478,7 +1511,7 @@
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" ht="16.5">
+    <row r="36" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A36" s="13"/>
       <c r="B36" s="3"/>
       <c r="C36" s="6"/>
@@ -1487,7 +1520,7 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" ht="16.5">
+    <row r="37" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A37" s="13"/>
       <c r="B37" s="3"/>
       <c r="C37" s="6"/>
@@ -1496,7 +1529,7 @@
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="1:7" ht="16.5">
+    <row r="38" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A38" s="13"/>
       <c r="B38" s="3"/>
       <c r="C38" s="6"/>
@@ -1505,7 +1538,7 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" ht="16.5">
+    <row r="39" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A39" s="13"/>
       <c r="B39" s="3"/>
       <c r="C39" s="6"/>
@@ -1514,7 +1547,7 @@
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:7" ht="16.5">
+    <row r="40" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A40" s="13"/>
       <c r="B40" s="3"/>
       <c r="C40" s="6"/>
@@ -1523,7 +1556,7 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41" s="14"/>
       <c r="B41" s="4"/>
       <c r="C41" s="7"/>
@@ -1532,7 +1565,7 @@
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42" s="12"/>
       <c r="B42" s="2"/>
       <c r="C42" s="5"/>
@@ -1545,7 +1578,7 @@
   <autoFilter ref="A1:G9"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -1556,7 +1589,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1569,7 +1602,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check in test issue list
</commit_message>
<xml_diff>
--- a/Docs/Testing Issue List.xlsx
+++ b/Docs/Testing Issue List.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Zhongding.git\trunk\Docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="195" windowWidth="20115" windowHeight="7875"/>
+    <workbookView xWindow="240" yWindow="255" windowWidth="20115" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Issue List" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="59">
   <si>
     <t>#</t>
   </si>
@@ -154,17 +149,84 @@
   <si>
     <t>Hold</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>帐号维护，如右图，为何帐号无效？</t>
+  </si>
+  <si>
+    <t>待解决</t>
+  </si>
+  <si>
+    <t>供应商合同的删除按钮没有作用</t>
+  </si>
+  <si>
+    <t>货品维护</t>
+  </si>
+  <si>
+    <t>供应商的textbox 稍微放长些；
+货品管理中的供应商没有按照帐套筛选，显示了别的帐套的供应商数据。</t>
+  </si>
+  <si>
+    <t>货品管理</t>
+  </si>
+  <si>
+    <t>货品定价管理</t>
+  </si>
+  <si>
+    <t>用户填写了价格以后，没有点击保存，离开页面前，需要提示用户，没有保存价格信息，确定是否要离开页面。</t>
+  </si>
+  <si>
+    <t>货品编号列的宽度变窄一点，把备注调宽一些
+规格也可以调窄一些，把货品名称变宽些</t>
+  </si>
+  <si>
+    <t>是否提醒/提醒期限 这2列不要换行</t>
+  </si>
+  <si>
+    <t>货品证照信息管理里，点编辑一个证照，证照信息没有默认加载。</t>
+  </si>
+  <si>
+    <t>客户+商业单位 需要验证是否重复。</t>
+  </si>
+  <si>
+    <t>银行账户管理，有跟#22 一样的问题，加横杠的帐号无法保存。</t>
+  </si>
+  <si>
+    <t>大包协议维护</t>
+  </si>
+  <si>
+    <t>医院名称的textbox 太短了。</t>
+  </si>
+  <si>
+    <t>医院设置要放在任务设置上方。
+大包协议判断重复是根据：客户+货品+规格+医院
+所以在维护医院名称的时候，不能判断医院的名字已经重复。</t>
+  </si>
+  <si>
+    <t>部门维护</t>
+  </si>
+  <si>
+    <t>员工管理</t>
+  </si>
+  <si>
+    <t>加上按部门筛选员工的功能</t>
+  </si>
+  <si>
+    <t>部门经理dropdown 不能清空选项； 新增部门时，部门经理dropdown应该为空。</t>
+  </si>
+  <si>
+    <t>所属部门 dropdown 一旦选了选项不能清空，检查系统中所有dropdown，需要增加一个空选项，允许用户清空dropdown。另外，允许用户新增员工，不属于任何一个部门。</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -191,7 +253,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -280,7 +342,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -677,11 +739,239 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>107277</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>599104</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>2228850</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7927302" y="28917901"/>
+          <a:ext cx="4559002" cy="2162174"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>322658</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>2410380</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7848600" y="31127700"/>
+          <a:ext cx="8018858" cy="2400855"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>446385</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>4559</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7877174" y="33661350"/>
+          <a:ext cx="9333211" cy="3033509"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>541646</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>2294906</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7848599" y="37557076"/>
+          <a:ext cx="5189847" cy="2266330"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>2352675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>265527</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>3544</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7905750" y="39671625"/>
+          <a:ext cx="8514177" cy="2460994"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>170276</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1532459</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7877175" y="43233975"/>
+          <a:ext cx="4789901" cy="1475309"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -723,7 +1013,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -758,7 +1048,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -967,26 +1257,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35:E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.125" style="15" customWidth="1"/>
-    <col min="2" max="2" width="22.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="18.75" style="20" customWidth="1"/>
-    <col min="5" max="5" width="15.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="51.875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.125" style="1"/>
+    <col min="1" max="1" width="11.140625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="20" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="51.85546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1007,7 +1297,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="133.5" customHeight="1">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -1026,7 +1316,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="16.5">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -1045,7 +1335,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" ht="191.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="191.25" customHeight="1">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -1064,7 +1354,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="74.25" customHeight="1">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -1083,7 +1373,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:7" ht="217.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="217.5" customHeight="1">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -1102,7 +1392,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7" ht="172.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="172.5" customHeight="1">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -1121,7 +1411,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7" ht="243.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="243.75" customHeight="1">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -1138,7 +1428,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" ht="33" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="49.5">
       <c r="A9" s="13">
         <v>8</v>
       </c>
@@ -1155,8 +1445,10 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A10" s="13"/>
+    <row r="10" spans="1:7" ht="16.5">
+      <c r="A10" s="13">
+        <v>9</v>
+      </c>
       <c r="B10" s="9" t="s">
         <v>18</v>
       </c>
@@ -1174,8 +1466,10 @@
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A11" s="13"/>
+    <row r="11" spans="1:7" ht="16.5">
+      <c r="A11" s="13">
+        <v>10</v>
+      </c>
       <c r="B11" s="9" t="s">
         <v>18</v>
       </c>
@@ -1193,8 +1487,10 @@
       </c>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7" ht="33" x14ac:dyDescent="0.15">
-      <c r="A12" s="13"/>
+    <row r="12" spans="1:7" ht="33">
+      <c r="A12" s="13">
+        <v>11</v>
+      </c>
       <c r="B12" s="9" t="s">
         <v>18</v>
       </c>
@@ -1212,8 +1508,10 @@
       </c>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:7" ht="33" x14ac:dyDescent="0.15">
-      <c r="A13" s="13"/>
+    <row r="13" spans="1:7" ht="33">
+      <c r="A13" s="13">
+        <v>12</v>
+      </c>
       <c r="B13" s="9" t="s">
         <v>18</v>
       </c>
@@ -1231,8 +1529,10 @@
       </c>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:7" ht="66" x14ac:dyDescent="0.15">
-      <c r="A14" s="13"/>
+    <row r="14" spans="1:7" ht="66">
+      <c r="A14" s="13">
+        <v>13</v>
+      </c>
       <c r="B14" s="9" t="s">
         <v>18</v>
       </c>
@@ -1250,8 +1550,10 @@
       </c>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:7" ht="33" x14ac:dyDescent="0.15">
-      <c r="A15" s="13"/>
+    <row r="15" spans="1:7" ht="33">
+      <c r="A15" s="13">
+        <v>14</v>
+      </c>
       <c r="B15" s="9" t="s">
         <v>18</v>
       </c>
@@ -1269,8 +1571,10 @@
       </c>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A16" s="13"/>
+    <row r="16" spans="1:7" ht="16.5">
+      <c r="A16" s="13">
+        <v>15</v>
+      </c>
       <c r="B16" s="9" t="s">
         <v>18</v>
       </c>
@@ -1288,8 +1592,10 @@
       </c>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="1:7" ht="186.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="13"/>
+    <row r="17" spans="1:7" ht="186.75" customHeight="1">
+      <c r="A17" s="13">
+        <v>16</v>
+      </c>
       <c r="B17" s="9" t="s">
         <v>18</v>
       </c>
@@ -1307,8 +1613,10 @@
       </c>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" ht="216.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="13"/>
+    <row r="18" spans="1:7" ht="216.75" customHeight="1">
+      <c r="A18" s="13">
+        <v>17</v>
+      </c>
       <c r="B18" s="9" t="s">
         <v>18</v>
       </c>
@@ -1326,8 +1634,10 @@
       </c>
       <c r="G18" s="9"/>
     </row>
-    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A19" s="13"/>
+    <row r="19" spans="1:7" ht="16.5">
+      <c r="A19" s="13">
+        <v>18</v>
+      </c>
       <c r="B19" s="9" t="s">
         <v>29</v>
       </c>
@@ -1345,8 +1655,10 @@
       </c>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="1:7" ht="199.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="13"/>
+    <row r="20" spans="1:7" ht="199.5" customHeight="1">
+      <c r="A20" s="13">
+        <v>19</v>
+      </c>
       <c r="B20" s="9" t="s">
         <v>29</v>
       </c>
@@ -1362,8 +1674,10 @@
       </c>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="1:7" ht="163.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="13"/>
+    <row r="21" spans="1:7" ht="163.5" customHeight="1">
+      <c r="A21" s="13">
+        <v>20</v>
+      </c>
       <c r="B21" s="9" t="s">
         <v>31</v>
       </c>
@@ -1379,8 +1693,10 @@
       </c>
       <c r="G21" s="9"/>
     </row>
-    <row r="22" spans="1:7" ht="162" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="13"/>
+    <row r="22" spans="1:7" ht="162" customHeight="1">
+      <c r="A22" s="13">
+        <v>21</v>
+      </c>
       <c r="B22" s="9" t="s">
         <v>31</v>
       </c>
@@ -1394,133 +1710,273 @@
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
     </row>
-    <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A23" s="13"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="9"/>
+    <row r="23" spans="1:7" ht="178.5" customHeight="1">
+      <c r="A23" s="13">
+        <v>22</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="11">
+        <v>41976</v>
+      </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
     </row>
-    <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A24" s="13"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="9"/>
+    <row r="24" spans="1:7" ht="198" customHeight="1">
+      <c r="A24" s="13">
+        <v>23</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="11">
+        <v>41976</v>
+      </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A25" s="13"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="9"/>
+    <row r="25" spans="1:7" ht="240.75" customHeight="1">
+      <c r="A25" s="13">
+        <v>24</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="11">
+        <v>41976</v>
+      </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
     </row>
-    <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A26" s="13"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="9"/>
+    <row r="26" spans="1:7" ht="49.5">
+      <c r="A26" s="13">
+        <v>25</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="11">
+        <v>41976</v>
+      </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A27" s="13"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="9"/>
+    <row r="27" spans="1:7" ht="190.5" customHeight="1">
+      <c r="A27" s="13">
+        <v>26</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="11">
+        <v>41976</v>
+      </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A28" s="13"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="9"/>
+    <row r="28" spans="1:7" ht="188.25" customHeight="1">
+      <c r="A28" s="13">
+        <v>27</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="11">
+        <v>41976</v>
+      </c>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A29" s="13"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="9"/>
+    <row r="29" spans="1:7" ht="33">
+      <c r="A29" s="13">
+        <v>28</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="11">
+        <v>41976</v>
+      </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A30" s="13"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="9"/>
+    <row r="30" spans="1:7" ht="16.5">
+      <c r="A30" s="13">
+        <v>29</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="11">
+        <v>41976</v>
+      </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
     </row>
-    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A31" s="13"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="9"/>
+    <row r="31" spans="1:7" ht="33">
+      <c r="A31" s="13">
+        <v>30</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="11">
+        <v>41976</v>
+      </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
     </row>
-    <row r="32" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A32" s="13"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="9"/>
+    <row r="32" spans="1:7" ht="121.5" customHeight="1">
+      <c r="A32" s="13">
+        <v>31</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="11">
+        <v>41976</v>
+      </c>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
     </row>
-    <row r="33" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A33" s="13"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="9"/>
+    <row r="33" spans="1:7" ht="99">
+      <c r="A33" s="13">
+        <v>32</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="11">
+        <v>41976</v>
+      </c>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
     </row>
-    <row r="34" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A34" s="13"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="9"/>
+    <row r="34" spans="1:7" ht="49.5">
+      <c r="A34" s="13">
+        <v>33</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="11">
+        <v>41976</v>
+      </c>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
     </row>
-    <row r="35" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="13"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="3"/>
+    <row r="35" spans="1:7" ht="16.5">
+      <c r="A35" s="13">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" s="11">
+        <v>41976</v>
+      </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="13"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="3"/>
+    <row r="36" spans="1:7" ht="82.5">
+      <c r="A36" s="13">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" s="11">
+        <v>41976</v>
+      </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="16.5">
       <c r="A37" s="13"/>
       <c r="B37" s="3"/>
       <c r="C37" s="6"/>
@@ -1529,7 +1985,7 @@
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="16.5">
       <c r="A38" s="13"/>
       <c r="B38" s="3"/>
       <c r="C38" s="6"/>
@@ -1538,7 +1994,7 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="16.5">
       <c r="A39" s="13"/>
       <c r="B39" s="3"/>
       <c r="C39" s="6"/>
@@ -1547,32 +2003,23 @@
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="13"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A41" s="14"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A42" s="12"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
+    <row r="40" spans="1:7">
+      <c r="A40" s="14"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="12"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G9"/>
@@ -1589,7 +2036,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1602,7 +2049,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed bug for purchase functions
</commit_message>
<xml_diff>
--- a/Docs/Testing Issue List.xlsx
+++ b/Docs/Testing Issue List.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Zhongding.git\trunk\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="255" windowWidth="20115" windowHeight="7815" activeTab="1"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="75">
   <si>
     <t>#</t>
   </si>
@@ -255,38 +260,50 @@
     <t>采购订单的grid header 不要换行</t>
   </si>
   <si>
-    <t>待解决</t>
-  </si>
-  <si>
     <t>备注框在创建订单第一个步骤时，不要显示。
 因为用户在正式提交或暂存订单之前，备注应该是可以修改的。</t>
   </si>
   <si>
-    <t>将采购订单的备注和审核意见分开来显示。</t>
-  </si>
-  <si>
-    <t>采购订单列表，只有暂存和退回状态的订单才可以被删除</t>
+    <t>出纳用户点了确认支付以后，在订单列表页面仍然可以看到已经支付完成的订单，这个不正确。
+出纳只能看到待支付的订单。</t>
+  </si>
+  <si>
+    <t>已解决</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>修改：采购订单列表页面，订单新增和修改权限的用户可以查询到所有状态的订单，包括自己的和别人提交的。
 但用户只能修改和删除自己暂存的或退回的订单，其他状态的订单或其他人的订单，用户只能查看，不能修改和删除。
 拥有审核权限或支付权限的用户，只能看到待审核或待支付的订单
 拥有修改权限的用户，可以看到所有状态的订单，并可以修改。</t>
-  </si>
-  <si>
-    <t>出纳用户点了确认支付以后，在订单列表页面仍然可以看到已经支付完成的订单，这个不正确。
-出纳只能看到待支付的订单。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>将采购订单的备注和审核意见分开来显示。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>采购订单列表，只有暂存和退回状态的订单才可以被删除</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>已解决</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>已解决</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -313,7 +330,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -415,7 +432,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1073,8 +1090,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9001125" y="219076"/>
-          <a:ext cx="8828390" cy="2623994"/>
+          <a:off x="10277475" y="200026"/>
+          <a:ext cx="9952340" cy="2623994"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1125,7 +1142,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1167,7 +1184,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1202,7 +1219,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1418,19 +1435,19 @@
       <selection pane="bottomLeft" activeCell="G1" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="20" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="51.85546875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="22.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18.75" style="20" customWidth="1"/>
+    <col min="5" max="5" width="15.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="51.875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1451,7 +1468,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="133.5" customHeight="1">
+    <row r="2" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -1470,7 +1487,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" ht="16.5">
+    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -1489,7 +1506,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" ht="191.25" customHeight="1">
+    <row r="4" spans="1:7" ht="191.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -1508,7 +1525,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7" ht="74.25" customHeight="1">
+    <row r="5" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -1527,7 +1544,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:7" ht="217.5" customHeight="1">
+    <row r="6" spans="1:7" ht="217.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -1546,7 +1563,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7" ht="172.5" customHeight="1">
+    <row r="7" spans="1:7" ht="172.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -1565,7 +1582,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7" ht="243.75" customHeight="1">
+    <row r="8" spans="1:7" ht="243.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -1582,7 +1599,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" ht="49.5">
+    <row r="9" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A9" s="13">
         <v>8</v>
       </c>
@@ -1599,7 +1616,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" ht="16.5">
+    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A10" s="13">
         <v>9</v>
       </c>
@@ -1620,7 +1637,7 @@
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" ht="16.5">
+    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A11" s="13">
         <v>10</v>
       </c>
@@ -1641,7 +1658,7 @@
       </c>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7" ht="33">
+    <row r="12" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A12" s="13">
         <v>11</v>
       </c>
@@ -1662,7 +1679,7 @@
       </c>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:7" ht="33">
+    <row r="13" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A13" s="13">
         <v>12</v>
       </c>
@@ -1683,7 +1700,7 @@
       </c>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:7" ht="66">
+    <row r="14" spans="1:7" ht="66" x14ac:dyDescent="0.15">
       <c r="A14" s="13">
         <v>13</v>
       </c>
@@ -1704,7 +1721,7 @@
       </c>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:7" ht="33">
+    <row r="15" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A15" s="13">
         <v>14</v>
       </c>
@@ -1725,7 +1742,7 @@
       </c>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" ht="16.5">
+    <row r="16" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A16" s="13">
         <v>15</v>
       </c>
@@ -1746,7 +1763,7 @@
       </c>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="1:7" ht="186.75" customHeight="1">
+    <row r="17" spans="1:7" ht="186.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13">
         <v>16</v>
       </c>
@@ -1767,7 +1784,7 @@
       </c>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" ht="216.75" customHeight="1">
+    <row r="18" spans="1:7" ht="216.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="13">
         <v>17</v>
       </c>
@@ -1788,7 +1805,7 @@
       </c>
       <c r="G18" s="9"/>
     </row>
-    <row r="19" spans="1:7" ht="16.5">
+    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A19" s="13">
         <v>18</v>
       </c>
@@ -1809,7 +1826,7 @@
       </c>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="1:7" ht="199.5" customHeight="1">
+    <row r="20" spans="1:7" ht="199.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13">
         <v>19</v>
       </c>
@@ -1828,7 +1845,7 @@
       </c>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="1:7" ht="163.5" customHeight="1">
+    <row r="21" spans="1:7" ht="163.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="13">
         <v>20</v>
       </c>
@@ -1847,7 +1864,7 @@
       </c>
       <c r="G21" s="9"/>
     </row>
-    <row r="22" spans="1:7" ht="162" customHeight="1">
+    <row r="22" spans="1:7" ht="162" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="13">
         <v>21</v>
       </c>
@@ -1864,7 +1881,7 @@
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
     </row>
-    <row r="23" spans="1:7" ht="178.5" customHeight="1">
+    <row r="23" spans="1:7" ht="178.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="13">
         <v>22</v>
       </c>
@@ -1885,7 +1902,7 @@
       </c>
       <c r="G23" s="9"/>
     </row>
-    <row r="24" spans="1:7" ht="198" customHeight="1">
+    <row r="24" spans="1:7" ht="198" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="13">
         <v>23</v>
       </c>
@@ -1906,7 +1923,7 @@
       </c>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="1:7" ht="240.75" customHeight="1">
+    <row r="25" spans="1:7" ht="240.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="13">
         <v>24</v>
       </c>
@@ -1927,7 +1944,7 @@
       </c>
       <c r="G25" s="9"/>
     </row>
-    <row r="26" spans="1:7" ht="49.5">
+    <row r="26" spans="1:7" ht="49.5" x14ac:dyDescent="0.15">
       <c r="A26" s="13">
         <v>25</v>
       </c>
@@ -1948,7 +1965,7 @@
       </c>
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="1:7" ht="190.5" customHeight="1">
+    <row r="27" spans="1:7" ht="190.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="13">
         <v>26</v>
       </c>
@@ -1969,7 +1986,7 @@
       </c>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="1:7" ht="188.25" customHeight="1">
+    <row r="28" spans="1:7" ht="188.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="13">
         <v>27</v>
       </c>
@@ -1990,7 +2007,7 @@
       </c>
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="1:7" ht="33">
+    <row r="29" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A29" s="13">
         <v>28</v>
       </c>
@@ -2011,7 +2028,7 @@
       </c>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="1:7" ht="16.5">
+    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A30" s="13">
         <v>29</v>
       </c>
@@ -2032,7 +2049,7 @@
       </c>
       <c r="G30" s="9"/>
     </row>
-    <row r="31" spans="1:7" ht="33">
+    <row r="31" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A31" s="13">
         <v>30</v>
       </c>
@@ -2053,7 +2070,7 @@
       </c>
       <c r="G31" s="9"/>
     </row>
-    <row r="32" spans="1:7" ht="121.5" customHeight="1">
+    <row r="32" spans="1:7" ht="121.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="13">
         <v>31</v>
       </c>
@@ -2074,7 +2091,7 @@
       </c>
       <c r="G32" s="9"/>
     </row>
-    <row r="33" spans="1:7" ht="99">
+    <row r="33" spans="1:7" ht="99" x14ac:dyDescent="0.15">
       <c r="A33" s="13">
         <v>32</v>
       </c>
@@ -2095,7 +2112,7 @@
       </c>
       <c r="G33" s="9"/>
     </row>
-    <row r="34" spans="1:7" ht="49.5">
+    <row r="34" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A34" s="13">
         <v>33</v>
       </c>
@@ -2116,7 +2133,7 @@
       </c>
       <c r="G34" s="9"/>
     </row>
-    <row r="35" spans="1:7" ht="16.5">
+    <row r="35" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A35" s="13">
         <v>34</v>
       </c>
@@ -2137,7 +2154,7 @@
       </c>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" ht="82.5">
+    <row r="36" spans="1:7" ht="66" x14ac:dyDescent="0.35">
       <c r="A36" s="13">
         <v>35</v>
       </c>
@@ -2158,7 +2175,7 @@
       </c>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" ht="16.5">
+    <row r="37" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A37" s="13"/>
       <c r="B37" s="3"/>
       <c r="C37" s="6"/>
@@ -2167,7 +2184,7 @@
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="1:7" ht="16.5">
+    <row r="38" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A38" s="13"/>
       <c r="B38" s="3"/>
       <c r="C38" s="6"/>
@@ -2176,7 +2193,7 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" ht="16.5">
+    <row r="39" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A39" s="13"/>
       <c r="B39" s="3"/>
       <c r="C39" s="6"/>
@@ -2185,7 +2202,7 @@
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40" s="14"/>
       <c r="B40" s="4"/>
       <c r="C40" s="7"/>
@@ -2194,7 +2211,7 @@
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41" s="12"/>
       <c r="B41" s="2"/>
       <c r="C41" s="5"/>
@@ -2216,22 +2233,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.875" customWidth="1"/>
+    <col min="2" max="2" width="15.875" customWidth="1"/>
     <col min="3" max="3" width="56" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.375" customWidth="1"/>
+    <col min="5" max="5" width="15.875" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="61.85546875" customWidth="1"/>
+    <col min="7" max="7" width="61.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -2252,7 +2269,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="210.75" customHeight="1">
+    <row r="2" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -2263,15 +2280,17 @@
         <v>66</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E2" s="24">
         <v>42008</v>
       </c>
-      <c r="F2" s="22"/>
+      <c r="F2" s="24">
+        <v>42019</v>
+      </c>
       <c r="G2" s="21"/>
     </row>
-    <row r="3" spans="1:7" ht="210.75" customHeight="1">
+    <row r="3" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="22">
         <v>2</v>
       </c>
@@ -2279,18 +2298,20 @@
         <v>65</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E3" s="24">
         <v>42008</v>
       </c>
-      <c r="F3" s="22"/>
+      <c r="F3" s="24">
+        <v>42019</v>
+      </c>
       <c r="G3" s="21"/>
     </row>
-    <row r="4" spans="1:7" ht="210.75" customHeight="1">
+    <row r="4" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="22">
         <v>3</v>
       </c>
@@ -2298,14 +2319,18 @@
         <v>65</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="22"/>
+        <v>67</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>69</v>
+      </c>
       <c r="E4" s="24"/>
-      <c r="F4" s="22"/>
+      <c r="F4" s="24">
+        <v>42019</v>
+      </c>
       <c r="G4" s="21"/>
     </row>
-    <row r="5" spans="1:7" ht="210.75" customHeight="1">
+    <row r="5" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="22">
         <v>4</v>
       </c>
@@ -2313,14 +2338,18 @@
         <v>65</v>
       </c>
       <c r="C5" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="22"/>
       <c r="E5" s="24"/>
-      <c r="F5" s="22"/>
+      <c r="F5" s="24">
+        <v>42019</v>
+      </c>
       <c r="G5" s="21"/>
     </row>
-    <row r="6" spans="1:7" ht="210.75" customHeight="1">
+    <row r="6" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="22">
         <v>5</v>
       </c>
@@ -2328,14 +2357,18 @@
         <v>65</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" s="22"/>
+        <v>72</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>74</v>
+      </c>
       <c r="E6" s="24"/>
-      <c r="F6" s="22"/>
+      <c r="F6" s="24">
+        <v>42019</v>
+      </c>
       <c r="G6" s="21"/>
     </row>
-    <row r="7" spans="1:7" ht="130.5" customHeight="1">
+    <row r="7" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="22">
         <v>6</v>
       </c>
@@ -2343,14 +2376,18 @@
         <v>65</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="22"/>
+        <v>68</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>69</v>
+      </c>
       <c r="E7" s="24"/>
-      <c r="F7" s="22"/>
+      <c r="F7" s="24">
+        <v>42019</v>
+      </c>
       <c r="G7" s="21"/>
     </row>
-    <row r="8" spans="1:7" ht="210.75" customHeight="1">
+    <row r="8" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="22"/>
       <c r="B8" s="22"/>
       <c r="C8" s="23"/>
@@ -2359,7 +2396,7 @@
       <c r="F8" s="22"/>
       <c r="G8" s="21"/>
     </row>
-    <row r="9" spans="1:7" ht="210.75" customHeight="1">
+    <row r="9" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="22"/>
       <c r="B9" s="22"/>
       <c r="C9" s="23"/>
@@ -2368,7 +2405,7 @@
       <c r="F9" s="22"/>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="1:7" ht="210.75" customHeight="1">
+    <row r="10" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="23"/>
@@ -2377,7 +2414,7 @@
       <c r="F10" s="22"/>
       <c r="G10" s="21"/>
     </row>
-    <row r="11" spans="1:7" ht="210.75" customHeight="1">
+    <row r="11" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="23"/>
@@ -2386,7 +2423,7 @@
       <c r="F11" s="22"/>
       <c r="G11" s="21"/>
     </row>
-    <row r="12" spans="1:7" ht="210.75" customHeight="1">
+    <row r="12" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="22"/>
       <c r="B12" s="22"/>
       <c r="C12" s="23"/>
@@ -2395,7 +2432,7 @@
       <c r="F12" s="22"/>
       <c r="G12" s="21"/>
     </row>
-    <row r="13" spans="1:7" ht="210.75" customHeight="1">
+    <row r="13" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="22"/>
       <c r="B13" s="22"/>
       <c r="C13" s="23"/>
@@ -2404,7 +2441,7 @@
       <c r="F13" s="22"/>
       <c r="G13" s="21"/>
     </row>
-    <row r="14" spans="1:7" ht="210.75" customHeight="1">
+    <row r="14" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="22"/>
       <c r="B14" s="22"/>
       <c r="C14" s="23"/>
@@ -2413,7 +2450,7 @@
       <c r="F14" s="22"/>
       <c r="G14" s="21"/>
     </row>
-    <row r="15" spans="1:7" ht="210.75" customHeight="1">
+    <row r="15" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="22"/>
       <c r="B15" s="22"/>
       <c r="C15" s="23"/>
@@ -2422,7 +2459,7 @@
       <c r="F15" s="22"/>
       <c r="G15" s="21"/>
     </row>
-    <row r="16" spans="1:7" ht="210.75" customHeight="1">
+    <row r="16" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="22"/>
       <c r="B16" s="22"/>
       <c r="C16" s="23"/>
@@ -2431,7 +2468,7 @@
       <c r="F16" s="22"/>
       <c r="G16" s="21"/>
     </row>
-    <row r="17" spans="1:7" ht="210.75" customHeight="1">
+    <row r="17" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="22"/>
       <c r="B17" s="22"/>
       <c r="C17" s="23"/>
@@ -2440,7 +2477,7 @@
       <c r="F17" s="22"/>
       <c r="G17" s="21"/>
     </row>
-    <row r="18" spans="1:7" ht="210.75" customHeight="1">
+    <row r="18" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="22"/>
       <c r="B18" s="22"/>
       <c r="C18" s="23"/>
@@ -2449,7 +2486,7 @@
       <c r="F18" s="22"/>
       <c r="G18" s="21"/>
     </row>
-    <row r="19" spans="1:7" ht="210.75" customHeight="1">
+    <row r="19" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="23"/>
@@ -2458,7 +2495,7 @@
       <c r="F19" s="22"/>
       <c r="G19" s="21"/>
     </row>
-    <row r="20" spans="1:7" ht="210.75" customHeight="1">
+    <row r="20" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="23"/>
@@ -2467,7 +2504,7 @@
       <c r="F20" s="22"/>
       <c r="G20" s="21"/>
     </row>
-    <row r="21" spans="1:7" ht="210.75" customHeight="1">
+    <row r="21" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="22"/>
       <c r="B21" s="22"/>
       <c r="C21" s="23"/>
@@ -2476,7 +2513,7 @@
       <c r="F21" s="22"/>
       <c r="G21" s="21"/>
     </row>
-    <row r="22" spans="1:7" ht="210.75" customHeight="1">
+    <row r="22" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="22"/>
       <c r="B22" s="22"/>
       <c r="C22" s="23"/>
@@ -2485,7 +2522,7 @@
       <c r="F22" s="22"/>
       <c r="G22" s="21"/>
     </row>
-    <row r="23" spans="1:7" ht="210.75" customHeight="1">
+    <row r="23" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="22"/>
       <c r="B23" s="22"/>
       <c r="C23" s="23"/>
@@ -2494,7 +2531,7 @@
       <c r="F23" s="22"/>
       <c r="G23" s="21"/>
     </row>
-    <row r="24" spans="1:7" ht="210.75" customHeight="1">
+    <row r="24" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="22"/>
       <c r="B24" s="22"/>
       <c r="C24" s="23"/>
@@ -2503,7 +2540,7 @@
       <c r="F24" s="22"/>
       <c r="G24" s="21"/>
     </row>
-    <row r="25" spans="1:7" ht="210.75" customHeight="1">
+    <row r="25" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="22"/>
       <c r="B25" s="22"/>
       <c r="C25" s="23"/>
@@ -2512,7 +2549,7 @@
       <c r="F25" s="22"/>
       <c r="G25" s="21"/>
     </row>
-    <row r="26" spans="1:7" ht="210.75" customHeight="1">
+    <row r="26" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="22"/>
       <c r="B26" s="22"/>
       <c r="C26" s="23"/>
@@ -2521,7 +2558,7 @@
       <c r="F26" s="22"/>
       <c r="G26" s="21"/>
     </row>
-    <row r="27" spans="1:7" ht="210.75" customHeight="1">
+    <row r="27" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="22"/>
       <c r="B27" s="22"/>
       <c r="C27" s="23"/>
@@ -2530,7 +2567,7 @@
       <c r="F27" s="22"/>
       <c r="G27" s="21"/>
     </row>
-    <row r="28" spans="1:7" ht="210.75" customHeight="1">
+    <row r="28" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="23"/>
@@ -2539,7 +2576,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="21"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29" s="21"/>
       <c r="B29" s="21"/>
       <c r="C29" s="21"/>
@@ -2548,7 +2585,7 @@
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30" s="21"/>
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
@@ -2557,7 +2594,7 @@
       <c r="F30" s="21"/>
       <c r="G30" s="21"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
@@ -2566,7 +2603,7 @@
       <c r="F31" s="21"/>
       <c r="G31" s="21"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" s="21"/>
       <c r="B32" s="21"/>
       <c r="C32" s="21"/>
@@ -2575,7 +2612,7 @@
       <c r="F32" s="21"/>
       <c r="G32" s="21"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -2584,7 +2621,7 @@
       <c r="F33" s="21"/>
       <c r="G33" s="21"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34" s="21"/>
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
@@ -2593,7 +2630,7 @@
       <c r="F34" s="21"/>
       <c r="G34" s="21"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
@@ -2602,7 +2639,7 @@
       <c r="F35" s="21"/>
       <c r="G35" s="21"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" s="21"/>
       <c r="B36" s="21"/>
       <c r="C36" s="21"/>
@@ -2611,7 +2648,7 @@
       <c r="F36" s="21"/>
       <c r="G36" s="21"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
@@ -2620,7 +2657,7 @@
       <c r="F37" s="21"/>
       <c r="G37" s="21"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" s="21"/>
       <c r="B38" s="21"/>
       <c r="C38" s="21"/>
@@ -2629,7 +2666,7 @@
       <c r="F38" s="21"/>
       <c r="G38" s="21"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="21"/>
@@ -2638,7 +2675,7 @@
       <c r="F39" s="21"/>
       <c r="G39" s="21"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40" s="21"/>
       <c r="B40" s="21"/>
       <c r="C40" s="21"/>
@@ -2647,7 +2684,7 @@
       <c r="F40" s="21"/>
       <c r="G40" s="21"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41" s="21"/>
       <c r="B41" s="21"/>
       <c r="C41" s="21"/>
@@ -2656,7 +2693,7 @@
       <c r="F41" s="21"/>
       <c r="G41" s="21"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42" s="21"/>
       <c r="B42" s="21"/>
       <c r="C42" s="21"/>
@@ -2665,7 +2702,7 @@
       <c r="F42" s="21"/>
       <c r="G42" s="21"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43" s="21"/>
       <c r="B43" s="21"/>
       <c r="C43" s="21"/>
@@ -2674,7 +2711,7 @@
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44" s="21"/>
       <c r="B44" s="21"/>
       <c r="C44" s="21"/>
@@ -2683,7 +2720,7 @@
       <c r="F44" s="21"/>
       <c r="G44" s="21"/>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45" s="21"/>
       <c r="B45" s="21"/>
       <c r="C45" s="21"/>
@@ -2692,7 +2729,7 @@
       <c r="F45" s="21"/>
       <c r="G45" s="21"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46" s="21"/>
       <c r="B46" s="21"/>
       <c r="C46" s="21"/>
@@ -2701,7 +2738,7 @@
       <c r="F46" s="21"/>
       <c r="G46" s="21"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A47" s="21"/>
       <c r="B47" s="21"/>
       <c r="C47" s="21"/>
@@ -2710,7 +2747,7 @@
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A48" s="21"/>
       <c r="B48" s="21"/>
       <c r="C48" s="21"/>
@@ -2719,7 +2756,7 @@
       <c r="F48" s="21"/>
       <c r="G48" s="21"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A49" s="21"/>
       <c r="B49" s="21"/>
       <c r="C49" s="21"/>
@@ -2728,7 +2765,7 @@
       <c r="F49" s="21"/>
       <c r="G49" s="21"/>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A50" s="21"/>
       <c r="B50" s="21"/>
       <c r="C50" s="21"/>
@@ -2737,7 +2774,7 @@
       <c r="F50" s="21"/>
       <c r="G50" s="21"/>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A51" s="21"/>
       <c r="B51" s="21"/>
       <c r="C51" s="21"/>
@@ -2746,7 +2783,7 @@
       <c r="F51" s="21"/>
       <c r="G51" s="21"/>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A52" s="21"/>
       <c r="B52" s="21"/>
       <c r="C52" s="21"/>
@@ -2755,7 +2792,7 @@
       <c r="F52" s="21"/>
       <c r="G52" s="21"/>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A53" s="21"/>
       <c r="B53" s="21"/>
       <c r="C53" s="21"/>
@@ -2764,7 +2801,7 @@
       <c r="F53" s="21"/>
       <c r="G53" s="21"/>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A54" s="21"/>
       <c r="B54" s="21"/>
       <c r="C54" s="21"/>
@@ -2773,7 +2810,7 @@
       <c r="F54" s="21"/>
       <c r="G54" s="21"/>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A55" s="21"/>
       <c r="B55" s="21"/>
       <c r="C55" s="21"/>
@@ -2782,7 +2819,7 @@
       <c r="F55" s="21"/>
       <c r="G55" s="21"/>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A56" s="21"/>
       <c r="B56" s="21"/>
       <c r="C56" s="21"/>
@@ -2791,7 +2828,7 @@
       <c r="F56" s="21"/>
       <c r="G56" s="21"/>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A57" s="21"/>
       <c r="B57" s="21"/>
       <c r="C57" s="21"/>
@@ -2800,7 +2837,7 @@
       <c r="F57" s="21"/>
       <c r="G57" s="21"/>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A58" s="21"/>
       <c r="B58" s="21"/>
       <c r="C58" s="21"/>
@@ -2809,7 +2846,7 @@
       <c r="F58" s="21"/>
       <c r="G58" s="21"/>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A59" s="21"/>
       <c r="B59" s="21"/>
       <c r="C59" s="21"/>
@@ -2818,7 +2855,7 @@
       <c r="F59" s="21"/>
       <c r="G59" s="21"/>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A60" s="21"/>
       <c r="B60" s="21"/>
       <c r="C60" s="21"/>
@@ -2827,7 +2864,7 @@
       <c r="F60" s="21"/>
       <c r="G60" s="21"/>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A61" s="21"/>
       <c r="B61" s="21"/>
       <c r="C61" s="21"/>
@@ -2836,7 +2873,7 @@
       <c r="F61" s="21"/>
       <c r="G61" s="21"/>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A62" s="21"/>
       <c r="B62" s="21"/>
       <c r="C62" s="21"/>
@@ -2845,7 +2882,7 @@
       <c r="F62" s="21"/>
       <c r="G62" s="21"/>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A63" s="21"/>
       <c r="B63" s="21"/>
       <c r="C63" s="21"/>
@@ -2854,7 +2891,7 @@
       <c r="F63" s="21"/>
       <c r="G63" s="21"/>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A64" s="21"/>
       <c r="B64" s="21"/>
       <c r="C64" s="21"/>
@@ -2863,7 +2900,7 @@
       <c r="F64" s="21"/>
       <c r="G64" s="21"/>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A65" s="21"/>
       <c r="B65" s="21"/>
       <c r="C65" s="21"/>
@@ -2872,7 +2909,7 @@
       <c r="F65" s="21"/>
       <c r="G65" s="21"/>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A66" s="21"/>
       <c r="B66" s="21"/>
       <c r="C66" s="21"/>
@@ -2881,7 +2918,7 @@
       <c r="F66" s="21"/>
       <c r="G66" s="21"/>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A67" s="21"/>
       <c r="B67" s="21"/>
       <c r="C67" s="21"/>
@@ -2890,7 +2927,7 @@
       <c r="F67" s="21"/>
       <c r="G67" s="21"/>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A68" s="21"/>
       <c r="B68" s="21"/>
       <c r="C68" s="21"/>
@@ -2899,7 +2936,7 @@
       <c r="F68" s="21"/>
       <c r="G68" s="21"/>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A69" s="21"/>
       <c r="B69" s="21"/>
       <c r="C69" s="21"/>
@@ -2908,7 +2945,7 @@
       <c r="F69" s="21"/>
       <c r="G69" s="21"/>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A70" s="21"/>
       <c r="B70" s="21"/>
       <c r="C70" s="21"/>
@@ -2917,7 +2954,7 @@
       <c r="F70" s="21"/>
       <c r="G70" s="21"/>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A71" s="21"/>
       <c r="B71" s="21"/>
       <c r="C71" s="21"/>
@@ -2926,7 +2963,7 @@
       <c r="F71" s="21"/>
       <c r="G71" s="21"/>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A72" s="21"/>
       <c r="B72" s="21"/>
       <c r="C72" s="21"/>
@@ -2935,7 +2972,7 @@
       <c r="F72" s="21"/>
       <c r="G72" s="21"/>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A73" s="21"/>
       <c r="B73" s="21"/>
       <c r="C73" s="21"/>
@@ -2944,7 +2981,7 @@
       <c r="F73" s="21"/>
       <c r="G73" s="21"/>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A74" s="21"/>
       <c r="B74" s="21"/>
       <c r="C74" s="21"/>
@@ -2953,7 +2990,7 @@
       <c r="F74" s="21"/>
       <c r="G74" s="21"/>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A75" s="21"/>
       <c r="B75" s="21"/>
       <c r="C75" s="21"/>
@@ -2962,7 +2999,7 @@
       <c r="F75" s="21"/>
       <c r="G75" s="21"/>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A76" s="21"/>
       <c r="B76" s="21"/>
       <c r="C76" s="21"/>
@@ -2971,7 +3008,7 @@
       <c r="F76" s="21"/>
       <c r="G76" s="21"/>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A77" s="21"/>
       <c r="B77" s="21"/>
       <c r="C77" s="21"/>
@@ -2983,7 +3020,8 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2993,7 +3031,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update issue list excel
</commit_message>
<xml_diff>
--- a/Docs/Testing Issue List.xlsx
+++ b/Docs/Testing Issue List.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Zhongding.git\trunk\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="315" windowWidth="20115" windowHeight="7755" activeTab="1"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="97">
   <si>
     <t>#</t>
   </si>
@@ -290,60 +295,100 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>待解决</t>
+  </si>
+  <si>
+    <t>入库单</t>
+  </si>
+  <si>
+    <t>入库单上的申请人，改为"操作人"</t>
+  </si>
+  <si>
+    <t>大包申请单</t>
+  </si>
+  <si>
+    <t>大包配送申请单</t>
+  </si>
+  <si>
+    <t>采购订单的货品没有按照帐套来筛选
+采购的货品列表应该根据帐套+供应商来筛选</t>
+  </si>
+  <si>
     <t>支付信息填写时，需要加一个验证，如果支付总金额大于或小于订单总金额，用户可以保存但不能提交。</t>
-  </si>
-  <si>
-    <t>待解决</t>
-  </si>
-  <si>
-    <t>入库单</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>已解决</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>入库单明细里，最后多了一列</t>
-  </si>
-  <si>
-    <t>入库单上的申请人，改为"操作人"</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>已解决</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>已解决</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>入库单，当货品入库的时候，现在会自动增加一条备注，这个不需要。 “入库单已入库（由系统自动生成）”</t>
-  </si>
-  <si>
-    <t>大包申请单</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>部门选项，应该显示跟当前申请人相关的部门</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>无需修改</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>已解决</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>业务经理没有数据加载，导致协议不能保存</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>大包配送申请单，删除列能不能不是单独的列？做为申请人，为什么不能删除申请单？</t>
-  </si>
-  <si>
-    <t>大包配送申请单</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>为什么只能看到2种货品？
 这里的货品，不要用业务经理来筛选，按部门筛选就可以了。</t>
-  </si>
-  <si>
-    <t>采购订单的货品没有按照帐套来筛选
-采购的货品列表应该根据帐套+供应商来筛选</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>具有审核权限的用户，没有看到审核按钮，只有查看
 最后一列的空白列是什么？</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>无需修改</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>无需修改</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>已解决</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -370,7 +415,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -472,7 +517,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1448,7 +1493,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1490,7 +1535,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1525,7 +1570,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1741,19 +1786,19 @@
       <selection pane="bottomLeft" activeCell="G1" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="20" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="51.85546875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="22.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18.75" style="20" customWidth="1"/>
+    <col min="5" max="5" width="15.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="51.875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1774,7 +1819,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="133.5" customHeight="1">
+    <row r="2" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -1793,7 +1838,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" ht="16.5">
+    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -1812,7 +1857,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" ht="191.25" customHeight="1">
+    <row r="4" spans="1:7" ht="191.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -1831,7 +1876,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7" ht="74.25" customHeight="1">
+    <row r="5" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -1850,7 +1895,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:7" ht="217.5" customHeight="1">
+    <row r="6" spans="1:7" ht="217.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -1869,7 +1914,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7" ht="172.5" customHeight="1">
+    <row r="7" spans="1:7" ht="172.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -1888,7 +1933,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7" ht="243.75" customHeight="1">
+    <row r="8" spans="1:7" ht="243.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -1905,7 +1950,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" ht="49.5">
+    <row r="9" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A9" s="13">
         <v>8</v>
       </c>
@@ -1922,7 +1967,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" ht="16.5">
+    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A10" s="13">
         <v>9</v>
       </c>
@@ -1943,7 +1988,7 @@
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" ht="16.5">
+    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A11" s="13">
         <v>10</v>
       </c>
@@ -1964,7 +2009,7 @@
       </c>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7" ht="33">
+    <row r="12" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A12" s="13">
         <v>11</v>
       </c>
@@ -1985,7 +2030,7 @@
       </c>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:7" ht="33">
+    <row r="13" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A13" s="13">
         <v>12</v>
       </c>
@@ -2006,7 +2051,7 @@
       </c>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:7" ht="66">
+    <row r="14" spans="1:7" ht="66" x14ac:dyDescent="0.15">
       <c r="A14" s="13">
         <v>13</v>
       </c>
@@ -2027,7 +2072,7 @@
       </c>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:7" ht="33">
+    <row r="15" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A15" s="13">
         <v>14</v>
       </c>
@@ -2048,7 +2093,7 @@
       </c>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" ht="16.5">
+    <row r="16" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A16" s="13">
         <v>15</v>
       </c>
@@ -2069,7 +2114,7 @@
       </c>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="1:7" ht="186.75" customHeight="1">
+    <row r="17" spans="1:7" ht="186.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13">
         <v>16</v>
       </c>
@@ -2090,7 +2135,7 @@
       </c>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" ht="216.75" customHeight="1">
+    <row r="18" spans="1:7" ht="216.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="13">
         <v>17</v>
       </c>
@@ -2111,7 +2156,7 @@
       </c>
       <c r="G18" s="9"/>
     </row>
-    <row r="19" spans="1:7" ht="16.5">
+    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A19" s="13">
         <v>18</v>
       </c>
@@ -2132,7 +2177,7 @@
       </c>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="1:7" ht="199.5" customHeight="1">
+    <row r="20" spans="1:7" ht="199.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13">
         <v>19</v>
       </c>
@@ -2151,7 +2196,7 @@
       </c>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="1:7" ht="163.5" customHeight="1">
+    <row r="21" spans="1:7" ht="163.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="13">
         <v>20</v>
       </c>
@@ -2170,7 +2215,7 @@
       </c>
       <c r="G21" s="9"/>
     </row>
-    <row r="22" spans="1:7" ht="162" customHeight="1">
+    <row r="22" spans="1:7" ht="162" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="13">
         <v>21</v>
       </c>
@@ -2187,7 +2232,7 @@
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
     </row>
-    <row r="23" spans="1:7" ht="178.5" customHeight="1">
+    <row r="23" spans="1:7" ht="178.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="13">
         <v>22</v>
       </c>
@@ -2208,7 +2253,7 @@
       </c>
       <c r="G23" s="9"/>
     </row>
-    <row r="24" spans="1:7" ht="198" customHeight="1">
+    <row r="24" spans="1:7" ht="198" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="13">
         <v>23</v>
       </c>
@@ -2229,7 +2274,7 @@
       </c>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="1:7" ht="240.75" customHeight="1">
+    <row r="25" spans="1:7" ht="240.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="13">
         <v>24</v>
       </c>
@@ -2250,7 +2295,7 @@
       </c>
       <c r="G25" s="9"/>
     </row>
-    <row r="26" spans="1:7" ht="49.5">
+    <row r="26" spans="1:7" ht="49.5" x14ac:dyDescent="0.15">
       <c r="A26" s="13">
         <v>25</v>
       </c>
@@ -2271,7 +2316,7 @@
       </c>
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="1:7" ht="190.5" customHeight="1">
+    <row r="27" spans="1:7" ht="190.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="13">
         <v>26</v>
       </c>
@@ -2292,7 +2337,7 @@
       </c>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="1:7" ht="188.25" customHeight="1">
+    <row r="28" spans="1:7" ht="188.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="13">
         <v>27</v>
       </c>
@@ -2313,7 +2358,7 @@
       </c>
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="1:7" ht="33">
+    <row r="29" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A29" s="13">
         <v>28</v>
       </c>
@@ -2334,7 +2379,7 @@
       </c>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="1:7" ht="16.5">
+    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A30" s="13">
         <v>29</v>
       </c>
@@ -2355,7 +2400,7 @@
       </c>
       <c r="G30" s="9"/>
     </row>
-    <row r="31" spans="1:7" ht="33">
+    <row r="31" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A31" s="13">
         <v>30</v>
       </c>
@@ -2376,7 +2421,7 @@
       </c>
       <c r="G31" s="9"/>
     </row>
-    <row r="32" spans="1:7" ht="121.5" customHeight="1">
+    <row r="32" spans="1:7" ht="121.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="13">
         <v>31</v>
       </c>
@@ -2397,7 +2442,7 @@
       </c>
       <c r="G32" s="9"/>
     </row>
-    <row r="33" spans="1:7" ht="99">
+    <row r="33" spans="1:7" ht="99" x14ac:dyDescent="0.15">
       <c r="A33" s="13">
         <v>32</v>
       </c>
@@ -2418,7 +2463,7 @@
       </c>
       <c r="G33" s="9"/>
     </row>
-    <row r="34" spans="1:7" ht="49.5">
+    <row r="34" spans="1:7" ht="33" x14ac:dyDescent="0.15">
       <c r="A34" s="13">
         <v>33</v>
       </c>
@@ -2439,7 +2484,7 @@
       </c>
       <c r="G34" s="9"/>
     </row>
-    <row r="35" spans="1:7" ht="16.5">
+    <row r="35" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A35" s="13">
         <v>34</v>
       </c>
@@ -2460,7 +2505,7 @@
       </c>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" ht="82.5">
+    <row r="36" spans="1:7" ht="66" x14ac:dyDescent="0.35">
       <c r="A36" s="13">
         <v>35</v>
       </c>
@@ -2481,7 +2526,7 @@
       </c>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" ht="16.5">
+    <row r="37" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A37" s="13"/>
       <c r="B37" s="3"/>
       <c r="C37" s="6"/>
@@ -2490,7 +2535,7 @@
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="1:7" ht="16.5">
+    <row r="38" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A38" s="13"/>
       <c r="B38" s="3"/>
       <c r="C38" s="6"/>
@@ -2499,7 +2544,7 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" ht="16.5">
+    <row r="39" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A39" s="13"/>
       <c r="B39" s="3"/>
       <c r="C39" s="6"/>
@@ -2508,7 +2553,7 @@
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40" s="14"/>
       <c r="B40" s="4"/>
       <c r="C40" s="7"/>
@@ -2517,7 +2562,7 @@
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41" s="12"/>
       <c r="B41" s="2"/>
       <c r="C41" s="5"/>
@@ -2539,22 +2584,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16:F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.875" customWidth="1"/>
+    <col min="2" max="2" width="15.875" customWidth="1"/>
     <col min="3" max="3" width="56" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.375" customWidth="1"/>
+    <col min="5" max="5" width="15.875" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="61.85546875" customWidth="1"/>
+    <col min="7" max="7" width="61.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -2575,7 +2621,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="210.75" customHeight="1">
+    <row r="2" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -2596,7 +2642,7 @@
       </c>
       <c r="G2" s="21"/>
     </row>
-    <row r="3" spans="1:7" ht="210.75" customHeight="1">
+    <row r="3" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="22">
         <v>2</v>
       </c>
@@ -2617,7 +2663,7 @@
       </c>
       <c r="G3" s="21"/>
     </row>
-    <row r="4" spans="1:7" ht="210.75" customHeight="1">
+    <row r="4" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="22">
         <v>3</v>
       </c>
@@ -2636,7 +2682,7 @@
       </c>
       <c r="G4" s="21"/>
     </row>
-    <row r="5" spans="1:7" ht="210.75" customHeight="1">
+    <row r="5" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="22">
         <v>4</v>
       </c>
@@ -2655,7 +2701,7 @@
       </c>
       <c r="G5" s="21"/>
     </row>
-    <row r="6" spans="1:7" ht="210.75" customHeight="1">
+    <row r="6" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="22">
         <v>5</v>
       </c>
@@ -2674,7 +2720,7 @@
       </c>
       <c r="G6" s="21"/>
     </row>
-    <row r="7" spans="1:7" ht="130.5" customHeight="1">
+    <row r="7" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="22">
         <v>6</v>
       </c>
@@ -2693,7 +2739,7 @@
       </c>
       <c r="G7" s="21"/>
     </row>
-    <row r="8" spans="1:7" ht="210.75" customHeight="1">
+    <row r="8" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="22">
         <v>7</v>
       </c>
@@ -2701,94 +2747,102 @@
         <v>65</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" s="24"/>
+        <v>82</v>
+      </c>
+      <c r="E8" s="24">
+        <v>42024</v>
+      </c>
       <c r="F8" s="24">
         <v>42024</v>
       </c>
       <c r="G8" s="21"/>
     </row>
-    <row r="9" spans="1:7" ht="210.75" customHeight="1">
+    <row r="9" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="22">
         <v>8</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="24"/>
+        <v>85</v>
+      </c>
+      <c r="E9" s="24">
+        <v>42024</v>
+      </c>
       <c r="F9" s="24">
         <v>42024</v>
       </c>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="22">
         <v>9</v>
       </c>
       <c r="B10" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="23" t="s">
-        <v>79</v>
-      </c>
       <c r="D10" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" s="24"/>
+        <v>84</v>
+      </c>
+      <c r="E10" s="24">
+        <v>42024</v>
+      </c>
       <c r="F10" s="24">
         <v>42024</v>
       </c>
       <c r="G10" s="21"/>
     </row>
-    <row r="11" spans="1:7" ht="30">
+    <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A11" s="22">
         <v>10</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" s="24"/>
+        <v>89</v>
+      </c>
+      <c r="E11" s="24">
+        <v>42024</v>
+      </c>
       <c r="F11" s="24">
         <v>42024</v>
       </c>
       <c r="G11" s="21"/>
     </row>
-    <row r="12" spans="1:7" ht="195" customHeight="1">
+    <row r="12" spans="1:7" ht="195" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="22">
         <v>11</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24">
+        <v>94</v>
+      </c>
+      <c r="E12" s="24">
         <v>42024</v>
       </c>
+      <c r="F12" s="24"/>
       <c r="G12" s="21"/>
     </row>
-    <row r="13" spans="1:7" ht="210.75" customHeight="1">
+    <row r="13" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="22">
         <v>12</v>
       </c>
@@ -2796,56 +2850,58 @@
         <v>47</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="24"/>
+        <v>57</v>
+      </c>
+      <c r="E13" s="24">
+        <v>42024</v>
+      </c>
       <c r="F13" s="24">
         <v>42024</v>
       </c>
       <c r="G13" s="21"/>
     </row>
-    <row r="14" spans="1:7" ht="210.75" customHeight="1">
+    <row r="14" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="22">
         <v>13</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24">
+        <v>88</v>
+      </c>
+      <c r="E14" s="24">
         <v>42024</v>
       </c>
+      <c r="F14" s="24"/>
       <c r="G14" s="21"/>
     </row>
-    <row r="15" spans="1:7" ht="195" customHeight="1">
+    <row r="15" spans="1:7" ht="195" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="22">
         <v>14</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24">
+        <v>75</v>
+      </c>
+      <c r="E15" s="24">
         <v>42024</v>
       </c>
+      <c r="F15" s="24"/>
       <c r="G15" s="21"/>
     </row>
-    <row r="16" spans="1:7" ht="210.75" customHeight="1">
+    <row r="16" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="22">
         <v>15</v>
       </c>
@@ -2853,37 +2909,39 @@
         <v>65</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="24"/>
+        <v>96</v>
+      </c>
+      <c r="E16" s="24">
+        <v>42024</v>
+      </c>
       <c r="F16" s="24">
         <v>42024</v>
       </c>
       <c r="G16" s="21"/>
     </row>
-    <row r="17" spans="1:7" ht="210.75" customHeight="1">
+    <row r="17" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="22">
         <v>16</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24">
+        <v>95</v>
+      </c>
+      <c r="E17" s="24">
         <v>42024</v>
       </c>
+      <c r="F17" s="24"/>
       <c r="G17" s="21"/>
     </row>
-    <row r="18" spans="1:7" ht="210.75" customHeight="1">
+    <row r="18" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="22">
         <v>17</v>
       </c>
@@ -2894,7 +2952,7 @@
       <c r="F18" s="22"/>
       <c r="G18" s="21"/>
     </row>
-    <row r="19" spans="1:7" ht="210.75" customHeight="1">
+    <row r="19" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="23"/>
@@ -2903,7 +2961,7 @@
       <c r="F19" s="22"/>
       <c r="G19" s="21"/>
     </row>
-    <row r="20" spans="1:7" ht="210.75" customHeight="1">
+    <row r="20" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="23"/>
@@ -2912,7 +2970,7 @@
       <c r="F20" s="22"/>
       <c r="G20" s="21"/>
     </row>
-    <row r="21" spans="1:7" ht="210.75" customHeight="1">
+    <row r="21" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="22"/>
       <c r="B21" s="22"/>
       <c r="C21" s="23"/>
@@ -2921,7 +2979,7 @@
       <c r="F21" s="22"/>
       <c r="G21" s="21"/>
     </row>
-    <row r="22" spans="1:7" ht="210.75" customHeight="1">
+    <row r="22" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="22"/>
       <c r="B22" s="22"/>
       <c r="C22" s="23"/>
@@ -2930,7 +2988,7 @@
       <c r="F22" s="22"/>
       <c r="G22" s="21"/>
     </row>
-    <row r="23" spans="1:7" ht="210.75" customHeight="1">
+    <row r="23" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="22"/>
       <c r="B23" s="22"/>
       <c r="C23" s="23"/>
@@ -2939,7 +2997,7 @@
       <c r="F23" s="22"/>
       <c r="G23" s="21"/>
     </row>
-    <row r="24" spans="1:7" ht="210.75" customHeight="1">
+    <row r="24" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="22"/>
       <c r="B24" s="22"/>
       <c r="C24" s="23"/>
@@ -2948,7 +3006,7 @@
       <c r="F24" s="22"/>
       <c r="G24" s="21"/>
     </row>
-    <row r="25" spans="1:7" ht="210.75" customHeight="1">
+    <row r="25" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="22"/>
       <c r="B25" s="22"/>
       <c r="C25" s="23"/>
@@ -2957,7 +3015,7 @@
       <c r="F25" s="22"/>
       <c r="G25" s="21"/>
     </row>
-    <row r="26" spans="1:7" ht="210.75" customHeight="1">
+    <row r="26" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="22"/>
       <c r="B26" s="22"/>
       <c r="C26" s="23"/>
@@ -2966,7 +3024,7 @@
       <c r="F26" s="22"/>
       <c r="G26" s="21"/>
     </row>
-    <row r="27" spans="1:7" ht="210.75" customHeight="1">
+    <row r="27" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="22"/>
       <c r="B27" s="22"/>
       <c r="C27" s="23"/>
@@ -2975,7 +3033,7 @@
       <c r="F27" s="22"/>
       <c r="G27" s="21"/>
     </row>
-    <row r="28" spans="1:7" ht="210.75" customHeight="1">
+    <row r="28" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="23"/>
@@ -2984,7 +3042,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="21"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29" s="21"/>
       <c r="B29" s="21"/>
       <c r="C29" s="21"/>
@@ -2993,7 +3051,7 @@
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30" s="21"/>
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
@@ -3002,7 +3060,7 @@
       <c r="F30" s="21"/>
       <c r="G30" s="21"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
@@ -3011,7 +3069,7 @@
       <c r="F31" s="21"/>
       <c r="G31" s="21"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" s="21"/>
       <c r="B32" s="21"/>
       <c r="C32" s="21"/>
@@ -3020,7 +3078,7 @@
       <c r="F32" s="21"/>
       <c r="G32" s="21"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -3029,7 +3087,7 @@
       <c r="F33" s="21"/>
       <c r="G33" s="21"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34" s="21"/>
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
@@ -3038,7 +3096,7 @@
       <c r="F34" s="21"/>
       <c r="G34" s="21"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
@@ -3047,7 +3105,7 @@
       <c r="F35" s="21"/>
       <c r="G35" s="21"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" s="21"/>
       <c r="B36" s="21"/>
       <c r="C36" s="21"/>
@@ -3056,7 +3114,7 @@
       <c r="F36" s="21"/>
       <c r="G36" s="21"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
@@ -3065,7 +3123,7 @@
       <c r="F37" s="21"/>
       <c r="G37" s="21"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" s="21"/>
       <c r="B38" s="21"/>
       <c r="C38" s="21"/>
@@ -3074,7 +3132,7 @@
       <c r="F38" s="21"/>
       <c r="G38" s="21"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="21"/>
@@ -3083,7 +3141,7 @@
       <c r="F39" s="21"/>
       <c r="G39" s="21"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40" s="21"/>
       <c r="B40" s="21"/>
       <c r="C40" s="21"/>
@@ -3092,7 +3150,7 @@
       <c r="F40" s="21"/>
       <c r="G40" s="21"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41" s="21"/>
       <c r="B41" s="21"/>
       <c r="C41" s="21"/>
@@ -3101,7 +3159,7 @@
       <c r="F41" s="21"/>
       <c r="G41" s="21"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42" s="21"/>
       <c r="B42" s="21"/>
       <c r="C42" s="21"/>
@@ -3110,7 +3168,7 @@
       <c r="F42" s="21"/>
       <c r="G42" s="21"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43" s="21"/>
       <c r="B43" s="21"/>
       <c r="C43" s="21"/>
@@ -3119,7 +3177,7 @@
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44" s="21"/>
       <c r="B44" s="21"/>
       <c r="C44" s="21"/>
@@ -3128,7 +3186,7 @@
       <c r="F44" s="21"/>
       <c r="G44" s="21"/>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45" s="21"/>
       <c r="B45" s="21"/>
       <c r="C45" s="21"/>
@@ -3137,7 +3195,7 @@
       <c r="F45" s="21"/>
       <c r="G45" s="21"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46" s="21"/>
       <c r="B46" s="21"/>
       <c r="C46" s="21"/>
@@ -3146,7 +3204,7 @@
       <c r="F46" s="21"/>
       <c r="G46" s="21"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A47" s="21"/>
       <c r="B47" s="21"/>
       <c r="C47" s="21"/>
@@ -3155,7 +3213,7 @@
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A48" s="21"/>
       <c r="B48" s="21"/>
       <c r="C48" s="21"/>
@@ -3164,7 +3222,7 @@
       <c r="F48" s="21"/>
       <c r="G48" s="21"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A49" s="21"/>
       <c r="B49" s="21"/>
       <c r="C49" s="21"/>
@@ -3173,7 +3231,7 @@
       <c r="F49" s="21"/>
       <c r="G49" s="21"/>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A50" s="21"/>
       <c r="B50" s="21"/>
       <c r="C50" s="21"/>
@@ -3182,7 +3240,7 @@
       <c r="F50" s="21"/>
       <c r="G50" s="21"/>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A51" s="21"/>
       <c r="B51" s="21"/>
       <c r="C51" s="21"/>
@@ -3191,7 +3249,7 @@
       <c r="F51" s="21"/>
       <c r="G51" s="21"/>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A52" s="21"/>
       <c r="B52" s="21"/>
       <c r="C52" s="21"/>
@@ -3200,7 +3258,7 @@
       <c r="F52" s="21"/>
       <c r="G52" s="21"/>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A53" s="21"/>
       <c r="B53" s="21"/>
       <c r="C53" s="21"/>
@@ -3209,7 +3267,7 @@
       <c r="F53" s="21"/>
       <c r="G53" s="21"/>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A54" s="21"/>
       <c r="B54" s="21"/>
       <c r="C54" s="21"/>
@@ -3218,7 +3276,7 @@
       <c r="F54" s="21"/>
       <c r="G54" s="21"/>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A55" s="21"/>
       <c r="B55" s="21"/>
       <c r="C55" s="21"/>
@@ -3227,7 +3285,7 @@
       <c r="F55" s="21"/>
       <c r="G55" s="21"/>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A56" s="21"/>
       <c r="B56" s="21"/>
       <c r="C56" s="21"/>
@@ -3236,7 +3294,7 @@
       <c r="F56" s="21"/>
       <c r="G56" s="21"/>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A57" s="21"/>
       <c r="B57" s="21"/>
       <c r="C57" s="21"/>
@@ -3245,7 +3303,7 @@
       <c r="F57" s="21"/>
       <c r="G57" s="21"/>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A58" s="21"/>
       <c r="B58" s="21"/>
       <c r="C58" s="21"/>
@@ -3254,7 +3312,7 @@
       <c r="F58" s="21"/>
       <c r="G58" s="21"/>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A59" s="21"/>
       <c r="B59" s="21"/>
       <c r="C59" s="21"/>
@@ -3263,7 +3321,7 @@
       <c r="F59" s="21"/>
       <c r="G59" s="21"/>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A60" s="21"/>
       <c r="B60" s="21"/>
       <c r="C60" s="21"/>
@@ -3272,7 +3330,7 @@
       <c r="F60" s="21"/>
       <c r="G60" s="21"/>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A61" s="21"/>
       <c r="B61" s="21"/>
       <c r="C61" s="21"/>
@@ -3281,7 +3339,7 @@
       <c r="F61" s="21"/>
       <c r="G61" s="21"/>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A62" s="21"/>
       <c r="B62" s="21"/>
       <c r="C62" s="21"/>
@@ -3290,7 +3348,7 @@
       <c r="F62" s="21"/>
       <c r="G62" s="21"/>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A63" s="21"/>
       <c r="B63" s="21"/>
       <c r="C63" s="21"/>
@@ -3299,7 +3357,7 @@
       <c r="F63" s="21"/>
       <c r="G63" s="21"/>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A64" s="21"/>
       <c r="B64" s="21"/>
       <c r="C64" s="21"/>
@@ -3308,7 +3366,7 @@
       <c r="F64" s="21"/>
       <c r="G64" s="21"/>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A65" s="21"/>
       <c r="B65" s="21"/>
       <c r="C65" s="21"/>
@@ -3317,7 +3375,7 @@
       <c r="F65" s="21"/>
       <c r="G65" s="21"/>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A66" s="21"/>
       <c r="B66" s="21"/>
       <c r="C66" s="21"/>
@@ -3326,7 +3384,7 @@
       <c r="F66" s="21"/>
       <c r="G66" s="21"/>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A67" s="21"/>
       <c r="B67" s="21"/>
       <c r="C67" s="21"/>
@@ -3335,7 +3393,7 @@
       <c r="F67" s="21"/>
       <c r="G67" s="21"/>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A68" s="21"/>
       <c r="B68" s="21"/>
       <c r="C68" s="21"/>
@@ -3344,7 +3402,7 @@
       <c r="F68" s="21"/>
       <c r="G68" s="21"/>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A69" s="21"/>
       <c r="B69" s="21"/>
       <c r="C69" s="21"/>
@@ -3353,7 +3411,7 @@
       <c r="F69" s="21"/>
       <c r="G69" s="21"/>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A70" s="21"/>
       <c r="B70" s="21"/>
       <c r="C70" s="21"/>
@@ -3362,7 +3420,7 @@
       <c r="F70" s="21"/>
       <c r="G70" s="21"/>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A71" s="21"/>
       <c r="B71" s="21"/>
       <c r="C71" s="21"/>
@@ -3371,7 +3429,7 @@
       <c r="F71" s="21"/>
       <c r="G71" s="21"/>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A72" s="21"/>
       <c r="B72" s="21"/>
       <c r="C72" s="21"/>
@@ -3380,7 +3438,7 @@
       <c r="F72" s="21"/>
       <c r="G72" s="21"/>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A73" s="21"/>
       <c r="B73" s="21"/>
       <c r="C73" s="21"/>
@@ -3389,7 +3447,7 @@
       <c r="F73" s="21"/>
       <c r="G73" s="21"/>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A74" s="21"/>
       <c r="B74" s="21"/>
       <c r="C74" s="21"/>
@@ -3398,7 +3456,7 @@
       <c r="F74" s="21"/>
       <c r="G74" s="21"/>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A75" s="21"/>
       <c r="B75" s="21"/>
       <c r="C75" s="21"/>
@@ -3407,7 +3465,7 @@
       <c r="F75" s="21"/>
       <c r="G75" s="21"/>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A76" s="21"/>
       <c r="B76" s="21"/>
       <c r="C76" s="21"/>
@@ -3416,7 +3474,7 @@
       <c r="F76" s="21"/>
       <c r="G76" s="21"/>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A77" s="21"/>
       <c r="B77" s="21"/>
       <c r="C77" s="21"/>
@@ -3439,7 +3497,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update testing issue list
</commit_message>
<xml_diff>
--- a/Docs/Testing Issue List.xlsx
+++ b/Docs/Testing Issue List.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Zhongding.git\trunk\Docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="435" windowWidth="20115" windowHeight="7635" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="435" windowWidth="20115" windowHeight="7635" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Issue List" sheetId="1" r:id="rId1"/>
     <sheet name="01-2015" sheetId="2" r:id="rId2"/>
     <sheet name="03-2015" sheetId="3" r:id="rId3"/>
+    <sheet name="05-2015" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Issue List'!$A$1:$G$9</definedName>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="122">
   <si>
     <t>#</t>
   </si>
@@ -410,16 +406,61 @@
     <t>采购单价没有预填</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t xml:space="preserve"> 待解决</t>
+  </si>
+  <si>
+    <t>负责人</t>
+  </si>
+  <si>
+    <t>Li Hong</t>
+  </si>
+  <si>
+    <t>grid中，header， 中止为什么比其他列的字小？</t>
+  </si>
+  <si>
+    <t>供应商余额抵扣功能需要考虑 - 需要讨论</t>
+  </si>
+  <si>
+    <t>将查询订单的功能，放在Grid上会更好，做成“+” 功能</t>
+  </si>
+  <si>
+    <t>入库单打印，格式有问题，列过宽， 可否将打印页面默认设为横向的？</t>
+  </si>
+  <si>
+    <t>入库单详情里，货品件数计算不正确
+小于1时，应该保留2位小数</t>
+  </si>
+  <si>
+    <t>支付完成，但未入库的订单，也应该允许用户中止订单</t>
+  </si>
+  <si>
+    <t>入库单的件数计算有误。 
+此产品，我在规格里配置为，每件50个，此处件数应为10，非20。
+同时，我更新了基本数量，件数没有相应变化</t>
+  </si>
+  <si>
+    <t>货品批号等信息都填写了，点击Grid上的保存，仍会提示。</t>
+  </si>
+  <si>
+    <t>把新增入库单，确认入库和修改入库单的权限分配给一个人， 此时，不能提交入库单，也不能确认入库</t>
+  </si>
+  <si>
+    <t>允许修改入库单权限用户，删除掉待入库的 入库单</t>
+  </si>
+  <si>
+    <t>当采购订单被中止，待入库的订单应该不允许用户 点击"确认入库"， 是否应该把状态改为“已中止”？</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -446,7 +487,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -460,7 +501,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -496,11 +537,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -582,9 +636,30 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1754,8 +1829,203 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>20959</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>103502</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1981200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10736584" y="200025"/>
+          <a:ext cx="4959343" cy="1971675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>485265</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1881400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10772775" y="2609851"/>
+          <a:ext cx="2256915" cy="1862349"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>284655</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1695243</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10772775" y="4543425"/>
+          <a:ext cx="8761905" cy="1657143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>12680</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>551289</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1581150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10728305" y="6448425"/>
+          <a:ext cx="6634609" cy="1590675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2381251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>551275</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1865441</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10706099" y="8839201"/>
+          <a:ext cx="6656801" cy="1874965"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1797,7 +2067,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1832,7 +2102,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2048,19 +2318,19 @@
       <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="22.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.625" style="26" customWidth="1"/>
-    <col min="4" max="4" width="18.75" style="16" customWidth="1"/>
-    <col min="5" max="5" width="15.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="51.875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.125" style="1"/>
+    <col min="1" max="1" width="11.140625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="16" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="51.85546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2081,7 +2351,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="133.5" customHeight="1">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -2102,7 +2372,7 @@
       </c>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="16.5">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -2121,7 +2391,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" ht="191.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="191.25" customHeight="1">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -2142,7 +2412,7 @@
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="74.25" customHeight="1">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -2163,7 +2433,7 @@
       </c>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:7" ht="217.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="217.5" customHeight="1">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -2184,7 +2454,7 @@
       </c>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:7" ht="172.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="172.5" customHeight="1">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -2205,7 +2475,7 @@
       </c>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" ht="243.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="243.75" customHeight="1">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -2222,7 +2492,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" ht="33" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="49.5">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -2239,7 +2509,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="16.5">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -2260,7 +2530,7 @@
       </c>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="16.5">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -2281,7 +2551,7 @@
       </c>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:7" ht="33" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="33">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -2302,7 +2572,7 @@
       </c>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:7" ht="33" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="33">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -2323,7 +2593,7 @@
       </c>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:7" ht="66" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="66">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -2344,7 +2614,7 @@
       </c>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:7" ht="33" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="33">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -2365,7 +2635,7 @@
       </c>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="16.5">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -2386,7 +2656,7 @@
       </c>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:7" ht="186.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="186.75" customHeight="1">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -2407,7 +2677,7 @@
       </c>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="1:7" ht="216.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="216.75" customHeight="1">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -2428,7 +2698,7 @@
       </c>
       <c r="G18" s="6"/>
     </row>
-    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="16.5">
       <c r="A19" s="9">
         <v>18</v>
       </c>
@@ -2449,7 +2719,7 @@
       </c>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="1:7" ht="199.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="199.5" customHeight="1">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -2468,7 +2738,7 @@
       </c>
       <c r="G20" s="6"/>
     </row>
-    <row r="21" spans="1:7" ht="163.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="163.5" customHeight="1">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -2487,7 +2757,7 @@
       </c>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="1:7" ht="162" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="162" customHeight="1">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -2504,7 +2774,7 @@
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
     </row>
-    <row r="23" spans="1:7" ht="178.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="178.5" customHeight="1">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -2525,7 +2795,7 @@
       </c>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="1:7" ht="198" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="198" customHeight="1">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -2546,7 +2816,7 @@
       </c>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="1:7" ht="240.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="240.75" customHeight="1">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -2567,7 +2837,7 @@
       </c>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="1:7" ht="49.5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="49.5">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -2588,7 +2858,7 @@
       </c>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:7" ht="190.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="190.5" customHeight="1">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -2609,7 +2879,7 @@
       </c>
       <c r="G27" s="6"/>
     </row>
-    <row r="28" spans="1:7" ht="188.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" ht="188.25" customHeight="1">
       <c r="A28" s="9">
         <v>27</v>
       </c>
@@ -2630,7 +2900,7 @@
       </c>
       <c r="G28" s="6"/>
     </row>
-    <row r="29" spans="1:7" ht="33" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" ht="33">
       <c r="A29" s="9">
         <v>28</v>
       </c>
@@ -2651,7 +2921,7 @@
       </c>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:7" ht="16.5">
       <c r="A30" s="9">
         <v>29</v>
       </c>
@@ -2672,7 +2942,7 @@
       </c>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="1:7" ht="33" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:7" ht="33">
       <c r="A31" s="9">
         <v>30</v>
       </c>
@@ -2693,7 +2963,7 @@
       </c>
       <c r="G31" s="6"/>
     </row>
-    <row r="32" spans="1:7" ht="121.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:7" ht="121.5" customHeight="1">
       <c r="A32" s="9">
         <v>31</v>
       </c>
@@ -2714,7 +2984,7 @@
       </c>
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="1:7" ht="99" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:7" ht="99">
       <c r="A33" s="9">
         <v>32</v>
       </c>
@@ -2735,7 +3005,7 @@
       </c>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="1:7" ht="33" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:7" ht="49.5">
       <c r="A34" s="9">
         <v>33</v>
       </c>
@@ -2756,7 +3026,7 @@
       </c>
       <c r="G34" s="6"/>
     </row>
-    <row r="35" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="16.5">
       <c r="A35" s="9">
         <v>34</v>
       </c>
@@ -2777,7 +3047,7 @@
       </c>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" ht="49.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="66">
       <c r="A36" s="9">
         <v>35</v>
       </c>
@@ -2798,7 +3068,7 @@
       </c>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" ht="207" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="207" customHeight="1">
       <c r="A37" s="9"/>
       <c r="B37" s="22"/>
       <c r="C37" s="24"/>
@@ -2807,7 +3077,7 @@
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="16.5">
       <c r="A38" s="9"/>
       <c r="B38" s="3"/>
       <c r="C38" s="24"/>
@@ -2816,7 +3086,7 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="16.5">
       <c r="A39" s="9"/>
       <c r="B39" s="3"/>
       <c r="C39" s="24"/>
@@ -2825,7 +3095,7 @@
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:7">
       <c r="A40" s="10"/>
       <c r="B40" s="4"/>
       <c r="C40" s="25"/>
@@ -2834,7 +3104,7 @@
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:7">
       <c r="A41" s="8"/>
       <c r="B41" s="2"/>
       <c r="C41" s="23"/>
@@ -2861,18 +3131,18 @@
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.875" customWidth="1"/>
-    <col min="2" max="2" width="15.875" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="3" width="56" customWidth="1"/>
-    <col min="4" max="4" width="15.375" customWidth="1"/>
-    <col min="5" max="5" width="15.875" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="61.875" customWidth="1"/>
+    <col min="7" max="7" width="61.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2893,7 +3163,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="210.75" customHeight="1">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -2914,7 +3184,7 @@
       </c>
       <c r="G2" s="17"/>
     </row>
-    <row r="3" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="210.75" customHeight="1">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -2935,7 +3205,7 @@
       </c>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="210.75" customHeight="1">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -2954,7 +3224,7 @@
       </c>
       <c r="G4" s="17"/>
     </row>
-    <row r="5" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="210.75" customHeight="1">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -2973,7 +3243,7 @@
       </c>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="210.75" customHeight="1">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -2992,7 +3262,7 @@
       </c>
       <c r="G6" s="17"/>
     </row>
-    <row r="7" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="130.5" customHeight="1">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -3011,7 +3281,7 @@
       </c>
       <c r="G7" s="17"/>
     </row>
-    <row r="8" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="210.75" customHeight="1">
       <c r="A8" s="18">
         <v>7</v>
       </c>
@@ -3032,7 +3302,7 @@
       </c>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="210.75" customHeight="1">
       <c r="A9" s="18">
         <v>8</v>
       </c>
@@ -3053,7 +3323,7 @@
       </c>
       <c r="G9" s="17"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7">
       <c r="A10" s="18">
         <v>9</v>
       </c>
@@ -3074,7 +3344,7 @@
       </c>
       <c r="G10" s="17"/>
     </row>
-    <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="30">
       <c r="A11" s="18">
         <v>10</v>
       </c>
@@ -3095,7 +3365,7 @@
       </c>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:7" ht="195" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="195" customHeight="1">
       <c r="A12" s="18">
         <v>11</v>
       </c>
@@ -3114,7 +3384,7 @@
       <c r="F12" s="20"/>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="210.75" customHeight="1">
       <c r="A13" s="18">
         <v>12</v>
       </c>
@@ -3135,7 +3405,7 @@
       </c>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="210.75" customHeight="1">
       <c r="A14" s="18">
         <v>13</v>
       </c>
@@ -3154,7 +3424,7 @@
       <c r="F14" s="20"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:7" ht="195" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="195" customHeight="1">
       <c r="A15" s="18">
         <v>14</v>
       </c>
@@ -3173,7 +3443,7 @@
       <c r="F15" s="20"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="210.75" customHeight="1">
       <c r="A16" s="18">
         <v>15</v>
       </c>
@@ -3194,7 +3464,7 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="210.75" customHeight="1">
       <c r="A17" s="18">
         <v>16</v>
       </c>
@@ -3213,7 +3483,7 @@
       <c r="F17" s="20"/>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="210.75" customHeight="1">
       <c r="A18" s="18">
         <v>17</v>
       </c>
@@ -3224,7 +3494,7 @@
       <c r="F18" s="18"/>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="210.75" customHeight="1">
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
       <c r="C19" s="19"/>
@@ -3233,7 +3503,7 @@
       <c r="F19" s="18"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="210.75" customHeight="1">
       <c r="A20" s="18"/>
       <c r="B20" s="18"/>
       <c r="C20" s="19"/>
@@ -3242,7 +3512,7 @@
       <c r="F20" s="18"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="210.75" customHeight="1">
       <c r="A21" s="18"/>
       <c r="B21" s="18"/>
       <c r="C21" s="19"/>
@@ -3251,7 +3521,7 @@
       <c r="F21" s="18"/>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="210.75" customHeight="1">
       <c r="A22" s="18"/>
       <c r="B22" s="18"/>
       <c r="C22" s="19"/>
@@ -3260,7 +3530,7 @@
       <c r="F22" s="18"/>
       <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="210.75" customHeight="1">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="19"/>
@@ -3269,7 +3539,7 @@
       <c r="F23" s="18"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="210.75" customHeight="1">
       <c r="A24" s="18"/>
       <c r="B24" s="18"/>
       <c r="C24" s="19"/>
@@ -3278,7 +3548,7 @@
       <c r="F24" s="18"/>
       <c r="G24" s="17"/>
     </row>
-    <row r="25" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="210.75" customHeight="1">
       <c r="A25" s="18"/>
       <c r="B25" s="18"/>
       <c r="C25" s="19"/>
@@ -3287,7 +3557,7 @@
       <c r="F25" s="18"/>
       <c r="G25" s="17"/>
     </row>
-    <row r="26" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="210.75" customHeight="1">
       <c r="A26" s="18"/>
       <c r="B26" s="18"/>
       <c r="C26" s="19"/>
@@ -3296,7 +3566,7 @@
       <c r="F26" s="18"/>
       <c r="G26" s="17"/>
     </row>
-    <row r="27" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="210.75" customHeight="1">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="19"/>
@@ -3305,7 +3575,7 @@
       <c r="F27" s="18"/>
       <c r="G27" s="17"/>
     </row>
-    <row r="28" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" ht="210.75" customHeight="1">
       <c r="A28" s="18"/>
       <c r="B28" s="18"/>
       <c r="C28" s="19"/>
@@ -3314,7 +3584,7 @@
       <c r="F28" s="18"/>
       <c r="G28" s="17"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7">
       <c r="A29" s="17"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
@@ -3323,7 +3593,7 @@
       <c r="F29" s="17"/>
       <c r="G29" s="17"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:7">
       <c r="A30" s="17"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
@@ -3332,7 +3602,7 @@
       <c r="F30" s="17"/>
       <c r="G30" s="17"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:7">
       <c r="A31" s="17"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -3341,7 +3611,7 @@
       <c r="F31" s="17"/>
       <c r="G31" s="17"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:7">
       <c r="A32" s="17"/>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -3350,7 +3620,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:7">
       <c r="A33" s="17"/>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
@@ -3359,7 +3629,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:7">
       <c r="A34" s="17"/>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
@@ -3368,7 +3638,7 @@
       <c r="F34" s="17"/>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:7">
       <c r="A35" s="17"/>
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
@@ -3377,7 +3647,7 @@
       <c r="F35" s="17"/>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:7">
       <c r="A36" s="17"/>
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
@@ -3386,7 +3656,7 @@
       <c r="F36" s="17"/>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:7">
       <c r="A37" s="17"/>
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
@@ -3395,7 +3665,7 @@
       <c r="F37" s="17"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:7">
       <c r="A38" s="17"/>
       <c r="B38" s="17"/>
       <c r="C38" s="17"/>
@@ -3404,7 +3674,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:7">
       <c r="A39" s="17"/>
       <c r="B39" s="17"/>
       <c r="C39" s="17"/>
@@ -3413,7 +3683,7 @@
       <c r="F39" s="17"/>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:7">
       <c r="A40" s="17"/>
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>
@@ -3422,7 +3692,7 @@
       <c r="F40" s="17"/>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:7">
       <c r="A41" s="17"/>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
@@ -3431,7 +3701,7 @@
       <c r="F41" s="17"/>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:7">
       <c r="A42" s="17"/>
       <c r="B42" s="17"/>
       <c r="C42" s="17"/>
@@ -3440,7 +3710,7 @@
       <c r="F42" s="17"/>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:7">
       <c r="A43" s="17"/>
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
@@ -3449,7 +3719,7 @@
       <c r="F43" s="17"/>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:7">
       <c r="A44" s="17"/>
       <c r="B44" s="17"/>
       <c r="C44" s="17"/>
@@ -3458,7 +3728,7 @@
       <c r="F44" s="17"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:7">
       <c r="A45" s="17"/>
       <c r="B45" s="17"/>
       <c r="C45" s="17"/>
@@ -3467,7 +3737,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:7">
       <c r="A46" s="17"/>
       <c r="B46" s="17"/>
       <c r="C46" s="17"/>
@@ -3476,7 +3746,7 @@
       <c r="F46" s="17"/>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:7">
       <c r="A47" s="17"/>
       <c r="B47" s="17"/>
       <c r="C47" s="17"/>
@@ -3485,7 +3755,7 @@
       <c r="F47" s="17"/>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:7">
       <c r="A48" s="17"/>
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
@@ -3494,7 +3764,7 @@
       <c r="F48" s="17"/>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:7">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
       <c r="C49" s="17"/>
@@ -3503,7 +3773,7 @@
       <c r="F49" s="17"/>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:7">
       <c r="A50" s="17"/>
       <c r="B50" s="17"/>
       <c r="C50" s="17"/>
@@ -3512,7 +3782,7 @@
       <c r="F50" s="17"/>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:7">
       <c r="A51" s="17"/>
       <c r="B51" s="17"/>
       <c r="C51" s="17"/>
@@ -3521,7 +3791,7 @@
       <c r="F51" s="17"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:7">
       <c r="A52" s="17"/>
       <c r="B52" s="17"/>
       <c r="C52" s="17"/>
@@ -3530,7 +3800,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:7">
       <c r="A53" s="17"/>
       <c r="B53" s="17"/>
       <c r="C53" s="17"/>
@@ -3539,7 +3809,7 @@
       <c r="F53" s="17"/>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:7">
       <c r="A54" s="17"/>
       <c r="B54" s="17"/>
       <c r="C54" s="17"/>
@@ -3548,7 +3818,7 @@
       <c r="F54" s="17"/>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:7">
       <c r="A55" s="17"/>
       <c r="B55" s="17"/>
       <c r="C55" s="17"/>
@@ -3557,7 +3827,7 @@
       <c r="F55" s="17"/>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:7">
       <c r="A56" s="17"/>
       <c r="B56" s="17"/>
       <c r="C56" s="17"/>
@@ -3566,7 +3836,7 @@
       <c r="F56" s="17"/>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:7">
       <c r="A57" s="17"/>
       <c r="B57" s="17"/>
       <c r="C57" s="17"/>
@@ -3575,7 +3845,7 @@
       <c r="F57" s="17"/>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:7">
       <c r="A58" s="17"/>
       <c r="B58" s="17"/>
       <c r="C58" s="17"/>
@@ -3584,7 +3854,7 @@
       <c r="F58" s="17"/>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:7">
       <c r="A59" s="17"/>
       <c r="B59" s="17"/>
       <c r="C59" s="17"/>
@@ -3593,7 +3863,7 @@
       <c r="F59" s="17"/>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:7">
       <c r="A60" s="17"/>
       <c r="B60" s="17"/>
       <c r="C60" s="17"/>
@@ -3602,7 +3872,7 @@
       <c r="F60" s="17"/>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:7">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
       <c r="C61" s="17"/>
@@ -3611,7 +3881,7 @@
       <c r="F61" s="17"/>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:7">
       <c r="A62" s="17"/>
       <c r="B62" s="17"/>
       <c r="C62" s="17"/>
@@ -3620,7 +3890,7 @@
       <c r="F62" s="17"/>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:7">
       <c r="A63" s="17"/>
       <c r="B63" s="17"/>
       <c r="C63" s="17"/>
@@ -3629,7 +3899,7 @@
       <c r="F63" s="17"/>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:7">
       <c r="A64" s="17"/>
       <c r="B64" s="17"/>
       <c r="C64" s="17"/>
@@ -3638,7 +3908,7 @@
       <c r="F64" s="17"/>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:7">
       <c r="A65" s="17"/>
       <c r="B65" s="17"/>
       <c r="C65" s="17"/>
@@ -3647,7 +3917,7 @@
       <c r="F65" s="17"/>
       <c r="G65" s="17"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:7">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
       <c r="C66" s="17"/>
@@ -3656,7 +3926,7 @@
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:7">
       <c r="A67" s="17"/>
       <c r="B67" s="17"/>
       <c r="C67" s="17"/>
@@ -3665,7 +3935,7 @@
       <c r="F67" s="17"/>
       <c r="G67" s="17"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:7">
       <c r="A68" s="17"/>
       <c r="B68" s="17"/>
       <c r="C68" s="17"/>
@@ -3674,7 +3944,7 @@
       <c r="F68" s="17"/>
       <c r="G68" s="17"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:7">
       <c r="A69" s="17"/>
       <c r="B69" s="17"/>
       <c r="C69" s="17"/>
@@ -3683,7 +3953,7 @@
       <c r="F69" s="17"/>
       <c r="G69" s="17"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:7">
       <c r="A70" s="17"/>
       <c r="B70" s="17"/>
       <c r="C70" s="17"/>
@@ -3692,7 +3962,7 @@
       <c r="F70" s="17"/>
       <c r="G70" s="17"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:7">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
       <c r="C71" s="17"/>
@@ -3701,7 +3971,7 @@
       <c r="F71" s="17"/>
       <c r="G71" s="17"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:7">
       <c r="A72" s="17"/>
       <c r="B72" s="17"/>
       <c r="C72" s="17"/>
@@ -3710,7 +3980,7 @@
       <c r="F72" s="17"/>
       <c r="G72" s="17"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:7">
       <c r="A73" s="17"/>
       <c r="B73" s="17"/>
       <c r="C73" s="17"/>
@@ -3719,7 +3989,7 @@
       <c r="F73" s="17"/>
       <c r="G73" s="17"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:7">
       <c r="A74" s="17"/>
       <c r="B74" s="17"/>
       <c r="C74" s="17"/>
@@ -3728,7 +3998,7 @@
       <c r="F74" s="17"/>
       <c r="G74" s="17"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:7">
       <c r="A75" s="17"/>
       <c r="B75" s="17"/>
       <c r="C75" s="17"/>
@@ -3737,7 +4007,7 @@
       <c r="F75" s="17"/>
       <c r="G75" s="17"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:7">
       <c r="A76" s="17"/>
       <c r="B76" s="17"/>
       <c r="C76" s="17"/>
@@ -3746,7 +4016,7 @@
       <c r="F76" s="17"/>
       <c r="G76" s="17"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:7">
       <c r="A77" s="17"/>
       <c r="B77" s="17"/>
       <c r="C77" s="17"/>
@@ -3767,21 +4037,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.75" style="30" customWidth="1"/>
-    <col min="3" max="3" width="86.125" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" style="30" customWidth="1"/>
-    <col min="5" max="5" width="11.875" style="30" customWidth="1"/>
-    <col min="6" max="6" width="10.625" customWidth="1"/>
-    <col min="7" max="7" width="49.375" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="30" customWidth="1"/>
+    <col min="3" max="3" width="86.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="30" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="30" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3801,7 +4071,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="84" customHeight="1">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -3821,7 +4091,7 @@
         <v>42076</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="176.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="176.25" customHeight="1">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -3841,7 +4111,7 @@
         <v>42076</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -3859,7 +4129,7 @@
         <v>42075</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -3877,7 +4147,7 @@
         <v>42075</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="90">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -3895,7 +4165,7 @@
         <v>42075</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="152.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="152.25" customHeight="1">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -3914,7 +4184,7 @@
       </c>
       <c r="G7" s="27"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7">
       <c r="A8" s="18">
         <v>7</v>
       </c>
@@ -3932,7 +4202,7 @@
         <v>42075</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="24" customHeight="1">
       <c r="A9" s="18">
         <v>8</v>
       </c>
@@ -3950,7 +4220,7 @@
         <v>42075</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="183" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="183" customHeight="1">
       <c r="A10" s="18">
         <v>9</v>
       </c>
@@ -3968,7 +4238,7 @@
         <v>42075</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7">
       <c r="A11" s="18">
         <v>10</v>
       </c>
@@ -3982,7 +4252,7 @@
       <c r="E11" s="29"/>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7">
       <c r="A12" s="18">
         <v>11</v>
       </c>
@@ -4000,7 +4270,7 @@
         <v>42075</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="54" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="60">
       <c r="A13" s="18">
         <v>12</v>
       </c>
@@ -4020,7 +4290,7 @@
         <v>42076</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="129" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="129" customHeight="1">
       <c r="A14" s="18">
         <v>13</v>
       </c>
@@ -4044,4 +4314,653 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="78.85546875" style="41" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="159" customHeight="1">
+      <c r="A2" s="37">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="20">
+        <v>42130</v>
+      </c>
+      <c r="F2" s="33"/>
+      <c r="G2" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="37">
+        <v>2</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="20">
+        <v>42130</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="37">
+        <v>3</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+    </row>
+    <row r="5" spans="1:7" ht="150.75" customHeight="1">
+      <c r="A5" s="37">
+        <v>4</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+    </row>
+    <row r="6" spans="1:7" ht="138.75" customHeight="1">
+      <c r="A6" s="37">
+        <v>5</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="17"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="37">
+        <v>6</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" spans="1:7" ht="188.25" customHeight="1">
+      <c r="A8" s="37">
+        <v>7</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:7" ht="158.25" customHeight="1">
+      <c r="A9" s="37">
+        <v>8</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="1:7" ht="30">
+      <c r="A10" s="37">
+        <v>9</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="37">
+        <v>10</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="17"/>
+    </row>
+    <row r="12" spans="1:7" ht="30">
+      <c r="A12" s="37">
+        <v>11</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="17"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="37"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="35"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="35"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="35"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="35"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="35"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="17"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="35"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="17"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="35"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="17"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="35"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="17"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="35"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="17"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="35"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="17"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="35"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="17"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="35"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="17"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="35"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="17"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="35"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="17"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="35"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="17"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="35"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="17"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="35"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="17"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="35"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="17"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="35"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="17"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="35"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="17"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="35"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="17"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="35"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="17"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="35"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="17"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="35"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="17"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="35"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="17"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="35"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="17"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="35"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="17"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="35"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="17"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="35"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="17"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="35"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="17"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="35"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="17"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="35"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="17"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="35"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="39"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="38"/>
+      <c r="G46" s="17"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="35"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="39"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="17"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="35"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="39"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="38"/>
+      <c r="F48" s="38"/>
+      <c r="G48" s="17"/>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="35"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="38"/>
+      <c r="F49" s="38"/>
+      <c r="G49" s="17"/>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="35"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="38"/>
+      <c r="E50" s="38"/>
+      <c r="F50" s="38"/>
+      <c r="G50" s="17"/>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="35"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="38"/>
+      <c r="E51" s="38"/>
+      <c r="F51" s="38"/>
+      <c r="G51" s="17"/>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="35"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="39"/>
+      <c r="D52" s="38"/>
+      <c r="E52" s="38"/>
+      <c r="F52" s="38"/>
+      <c r="G52" s="17"/>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="35"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="39"/>
+      <c r="D53" s="38"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="17"/>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="35"/>
+      <c r="B54" s="38"/>
+      <c r="C54" s="39"/>
+      <c r="D54" s="38"/>
+      <c r="E54" s="38"/>
+      <c r="F54" s="38"/>
+      <c r="G54" s="17"/>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="35"/>
+      <c r="B55" s="38"/>
+      <c r="C55" s="39"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="38"/>
+      <c r="F55" s="38"/>
+      <c r="G55" s="17"/>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="35"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="39"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="38"/>
+      <c r="F56" s="38"/>
+      <c r="G56" s="17"/>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="B57" s="17"/>
+      <c r="C57" s="40"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="B58" s="17"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="B59" s="17"/>
+      <c r="C59" s="40"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="B60" s="17"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>